<commit_message>
Worked on SQLite inp casting
sad. see blog notes
</commit_message>
<xml_diff>
--- a/Wknd_Sched_Builder/Long Weekend Polling.xlsx
+++ b/Wknd_Sched_Builder/Long Weekend Polling.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cloned_Repositories\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cloned_Repositories\HFS_Gradio_Projects\Wknd_Sched_Builder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79D41A1-58D9-4E31-AA8E-6834CF71EF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF50D8EA-8FA1-4826-BDFC-E19DD266A824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7068" yWindow="756" windowWidth="17700" windowHeight="11244" tabRatio="575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="12012" windowHeight="11196" tabRatio="575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -776,6 +776,18 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -785,37 +797,31 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -836,22 +842,16 @@
     <xf numFmtId="164" fontId="11" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -8062,8 +8062,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BH179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Q47" sqref="Q47"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8096,12 +8096,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:59" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="100" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
       <c r="E1" s="23"/>
       <c r="F1" s="23"/>
       <c r="G1" s="23"/>
@@ -8159,28 +8159,28 @@
       <c r="BG1" s="17"/>
     </row>
     <row r="2" spans="1:59" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
       <c r="E2" s="23"/>
-      <c r="F2" s="85" t="s">
+      <c r="F2" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="86" t="s">
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="87" t="s">
+      <c r="J2" s="90"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="87"/>
-      <c r="N2" s="87"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="91"/>
       <c r="O2" s="88" t="s">
         <v>19</v>
       </c>
@@ -8193,21 +8193,21 @@
       <c r="V2" s="23"/>
       <c r="W2" s="23"/>
       <c r="X2" s="23"/>
-      <c r="Y2" s="85" t="s">
+      <c r="Y2" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="Z2" s="85"/>
-      <c r="AA2" s="85"/>
-      <c r="AB2" s="86" t="s">
+      <c r="Z2" s="89"/>
+      <c r="AA2" s="89"/>
+      <c r="AB2" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="AC2" s="86"/>
-      <c r="AD2" s="86"/>
-      <c r="AE2" s="87" t="s">
+      <c r="AC2" s="90"/>
+      <c r="AD2" s="90"/>
+      <c r="AE2" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="AF2" s="87"/>
-      <c r="AG2" s="87"/>
+      <c r="AF2" s="91"/>
+      <c r="AG2" s="91"/>
       <c r="AH2" s="88" t="s">
         <v>19</v>
       </c>
@@ -8245,26 +8245,26 @@
       <c r="C3" s="98"/>
       <c r="D3" s="98"/>
       <c r="E3" s="27"/>
-      <c r="F3" s="89" t="s">
+      <c r="F3" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="90"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="89" t="s">
+      <c r="G3" s="86"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="90"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="89" t="s">
+      <c r="J3" s="86"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="90"/>
-      <c r="N3" s="91"/>
-      <c r="O3" s="89" t="s">
+      <c r="M3" s="86"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="90"/>
-      <c r="Q3" s="91"/>
+      <c r="P3" s="86"/>
+      <c r="Q3" s="87"/>
       <c r="R3" s="36"/>
       <c r="S3" s="37"/>
       <c r="T3" s="98" t="s">
@@ -8274,26 +8274,26 @@
       <c r="V3" s="98"/>
       <c r="W3" s="98"/>
       <c r="X3" s="24"/>
-      <c r="Y3" s="89" t="s">
+      <c r="Y3" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="Z3" s="90"/>
-      <c r="AA3" s="91"/>
-      <c r="AB3" s="89" t="s">
+      <c r="Z3" s="86"/>
+      <c r="AA3" s="87"/>
+      <c r="AB3" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="AC3" s="90"/>
-      <c r="AD3" s="91"/>
-      <c r="AE3" s="89" t="s">
+      <c r="AC3" s="86"/>
+      <c r="AD3" s="87"/>
+      <c r="AE3" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="90"/>
-      <c r="AG3" s="91"/>
-      <c r="AH3" s="89" t="s">
+      <c r="AF3" s="86"/>
+      <c r="AG3" s="87"/>
+      <c r="AH3" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="AI3" s="90"/>
-      <c r="AJ3" s="91"/>
+      <c r="AI3" s="86"/>
+      <c r="AJ3" s="87"/>
       <c r="AK3" s="36"/>
     </row>
     <row r="4" spans="1:59" s="17" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -8408,7 +8408,7 @@
       </c>
     </row>
     <row r="5" spans="1:59" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="105" t="s">
+      <c r="A5" s="92" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="53"/>
@@ -8429,7 +8429,7 @@
       <c r="Q5" s="29"/>
       <c r="R5" s="71"/>
       <c r="S5" s="10"/>
-      <c r="T5" s="105" t="s">
+      <c r="T5" s="92" t="s">
         <v>2</v>
       </c>
       <c r="U5" s="53"/>
@@ -8451,7 +8451,7 @@
       <c r="AK5" s="73"/>
     </row>
     <row r="6" spans="1:59" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="106"/>
+      <c r="A6" s="93"/>
       <c r="B6" s="44"/>
       <c r="C6" s="44"/>
       <c r="D6" s="45"/>
@@ -8470,7 +8470,7 @@
       <c r="Q6" s="29"/>
       <c r="R6" s="66"/>
       <c r="S6" s="39"/>
-      <c r="T6" s="106"/>
+      <c r="T6" s="93"/>
       <c r="U6" s="44"/>
       <c r="V6" s="44"/>
       <c r="W6" s="45"/>
@@ -8490,7 +8490,7 @@
       <c r="AK6" s="66"/>
     </row>
     <row r="7" spans="1:59" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="106"/>
+      <c r="A7" s="93"/>
       <c r="B7" s="44"/>
       <c r="C7" s="44"/>
       <c r="D7" s="45"/>
@@ -8509,7 +8509,7 @@
       <c r="Q7" s="29"/>
       <c r="R7" s="31"/>
       <c r="S7" s="39"/>
-      <c r="T7" s="106"/>
+      <c r="T7" s="93"/>
       <c r="U7" s="44"/>
       <c r="V7" s="44"/>
       <c r="W7" s="45"/>
@@ -8529,7 +8529,7 @@
       <c r="AK7" s="31"/>
     </row>
     <row r="8" spans="1:59" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="106"/>
+      <c r="A8" s="93"/>
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
       <c r="D8" s="44"/>
@@ -8548,7 +8548,7 @@
       <c r="Q8" s="29"/>
       <c r="R8" s="66"/>
       <c r="S8" s="39"/>
-      <c r="T8" s="106"/>
+      <c r="T8" s="93"/>
       <c r="U8" s="44"/>
       <c r="V8" s="44"/>
       <c r="W8" s="45"/>
@@ -8568,7 +8568,7 @@
       <c r="AK8" s="66"/>
     </row>
     <row r="9" spans="1:59" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="106"/>
+      <c r="A9" s="93"/>
       <c r="B9" s="44"/>
       <c r="C9" s="44"/>
       <c r="D9" s="45"/>
@@ -8587,7 +8587,7 @@
       <c r="Q9" s="29"/>
       <c r="R9" s="31"/>
       <c r="S9" s="39"/>
-      <c r="T9" s="106"/>
+      <c r="T9" s="93"/>
       <c r="U9" s="44"/>
       <c r="V9" s="44"/>
       <c r="W9" s="45"/>
@@ -8607,7 +8607,7 @@
       <c r="AK9" s="31"/>
     </row>
     <row r="10" spans="1:59" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="106"/>
+      <c r="A10" s="93"/>
       <c r="B10" s="44"/>
       <c r="C10" s="44"/>
       <c r="D10" s="44"/>
@@ -8626,7 +8626,7 @@
       <c r="Q10" s="29"/>
       <c r="R10" s="31"/>
       <c r="S10" s="39"/>
-      <c r="T10" s="106"/>
+      <c r="T10" s="93"/>
       <c r="U10" s="44"/>
       <c r="V10" s="44"/>
       <c r="W10" s="45"/>
@@ -8646,7 +8646,7 @@
       <c r="AK10" s="31"/>
     </row>
     <row r="11" spans="1:59" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="106"/>
+      <c r="A11" s="93"/>
       <c r="B11" s="48"/>
       <c r="C11" s="49"/>
       <c r="D11" s="49"/>
@@ -8665,7 +8665,7 @@
       <c r="Q11" s="29"/>
       <c r="R11" s="31"/>
       <c r="S11" s="39"/>
-      <c r="T11" s="106"/>
+      <c r="T11" s="93"/>
       <c r="U11" s="44"/>
       <c r="V11" s="44"/>
       <c r="W11" s="45"/>
@@ -8685,7 +8685,7 @@
       <c r="AK11" s="31"/>
     </row>
     <row r="12" spans="1:59" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="106"/>
+      <c r="A12" s="93"/>
       <c r="B12" s="47"/>
       <c r="C12" s="44"/>
       <c r="D12" s="45"/>
@@ -8704,7 +8704,7 @@
       <c r="Q12" s="29"/>
       <c r="R12" s="31"/>
       <c r="S12" s="39"/>
-      <c r="T12" s="106"/>
+      <c r="T12" s="93"/>
       <c r="U12" s="47"/>
       <c r="V12" s="44"/>
       <c r="W12" s="45"/>
@@ -8724,7 +8724,7 @@
       <c r="AK12" s="31"/>
     </row>
     <row r="13" spans="1:59" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="106"/>
+      <c r="A13" s="93"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -8743,7 +8743,7 @@
       <c r="Q13" s="29"/>
       <c r="R13" s="31"/>
       <c r="S13" s="39"/>
-      <c r="T13" s="106"/>
+      <c r="T13" s="93"/>
       <c r="U13" s="54"/>
       <c r="V13" s="52"/>
       <c r="W13" s="52"/>
@@ -8763,7 +8763,7 @@
       <c r="AK13" s="31"/>
     </row>
     <row r="14" spans="1:59" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="106"/>
+      <c r="A14" s="93"/>
       <c r="B14" s="44"/>
       <c r="C14" s="44"/>
       <c r="D14" s="45"/>
@@ -8782,7 +8782,7 @@
       <c r="Q14" s="29"/>
       <c r="R14" s="31"/>
       <c r="S14" s="39"/>
-      <c r="T14" s="106"/>
+      <c r="T14" s="93"/>
       <c r="U14" s="54"/>
       <c r="V14" s="52"/>
       <c r="W14" s="52"/>
@@ -8802,7 +8802,7 @@
       <c r="AK14" s="31"/>
     </row>
     <row r="15" spans="1:59" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="106"/>
+      <c r="A15" s="93"/>
       <c r="B15" s="48"/>
       <c r="C15" s="49"/>
       <c r="D15" s="49"/>
@@ -8821,7 +8821,7 @@
       <c r="Q15" s="29"/>
       <c r="R15" s="31"/>
       <c r="S15" s="39"/>
-      <c r="T15" s="106"/>
+      <c r="T15" s="93"/>
       <c r="U15" s="44"/>
       <c r="V15" s="44"/>
       <c r="W15" s="45"/>
@@ -8841,7 +8841,7 @@
       <c r="AK15" s="31"/>
     </row>
     <row r="16" spans="1:59" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="106"/>
+      <c r="A16" s="93"/>
       <c r="B16" s="44"/>
       <c r="C16" s="44"/>
       <c r="D16" s="44"/>
@@ -8860,7 +8860,7 @@
       <c r="Q16" s="29"/>
       <c r="R16" s="31"/>
       <c r="S16" s="39"/>
-      <c r="T16" s="106"/>
+      <c r="T16" s="93"/>
       <c r="U16" s="44"/>
       <c r="V16" s="44"/>
       <c r="W16" s="45"/>
@@ -8880,7 +8880,7 @@
       <c r="AK16" s="31"/>
     </row>
     <row r="17" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="106"/>
+      <c r="A17" s="93"/>
       <c r="B17" s="54"/>
       <c r="C17" s="49"/>
       <c r="D17" s="49"/>
@@ -8899,7 +8899,7 @@
       <c r="Q17" s="29"/>
       <c r="R17" s="31"/>
       <c r="S17" s="39"/>
-      <c r="T17" s="106"/>
+      <c r="T17" s="93"/>
       <c r="U17" s="54"/>
       <c r="V17" s="52"/>
       <c r="W17" s="52"/>
@@ -8919,7 +8919,7 @@
       <c r="AK17" s="31"/>
     </row>
     <row r="18" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="106"/>
+      <c r="A18" s="93"/>
       <c r="B18" s="54"/>
       <c r="C18" s="49"/>
       <c r="D18" s="49"/>
@@ -8938,7 +8938,7 @@
       <c r="Q18" s="29"/>
       <c r="R18" s="31"/>
       <c r="S18" s="39"/>
-      <c r="T18" s="106"/>
+      <c r="T18" s="93"/>
       <c r="U18" s="55"/>
       <c r="V18" s="44"/>
       <c r="W18" s="45"/>
@@ -8958,7 +8958,7 @@
       <c r="AK18" s="31"/>
     </row>
     <row r="19" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="106"/>
+      <c r="A19" s="93"/>
       <c r="B19" s="44"/>
       <c r="C19" s="44"/>
       <c r="D19" s="44"/>
@@ -8977,7 +8977,7 @@
       <c r="Q19" s="29"/>
       <c r="R19" s="31"/>
       <c r="S19" s="39"/>
-      <c r="T19" s="106"/>
+      <c r="T19" s="93"/>
       <c r="U19" s="44"/>
       <c r="V19" s="44"/>
       <c r="W19" s="45"/>
@@ -8997,7 +8997,7 @@
       <c r="AK19" s="31"/>
     </row>
     <row r="20" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="106"/>
+      <c r="A20" s="93"/>
       <c r="B20" s="55"/>
       <c r="C20" s="44"/>
       <c r="D20" s="45"/>
@@ -9016,7 +9016,7 @@
       <c r="Q20" s="29"/>
       <c r="R20" s="31"/>
       <c r="S20" s="39"/>
-      <c r="T20" s="106"/>
+      <c r="T20" s="93"/>
       <c r="U20" s="44"/>
       <c r="V20" s="44"/>
       <c r="W20" s="45"/>
@@ -9036,7 +9036,7 @@
       <c r="AK20" s="31"/>
     </row>
     <row r="21" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="106"/>
+      <c r="A21" s="93"/>
       <c r="B21" s="44"/>
       <c r="C21" s="44"/>
       <c r="D21" s="45"/>
@@ -9055,7 +9055,7 @@
       <c r="Q21" s="29"/>
       <c r="R21" s="31"/>
       <c r="S21" s="39"/>
-      <c r="T21" s="106"/>
+      <c r="T21" s="93"/>
       <c r="U21" s="55"/>
       <c r="V21" s="44"/>
       <c r="W21" s="45"/>
@@ -9075,7 +9075,7 @@
       <c r="AK21" s="31"/>
     </row>
     <row r="22" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="106"/>
+      <c r="A22" s="93"/>
       <c r="B22" s="44"/>
       <c r="C22" s="44"/>
       <c r="D22" s="45"/>
@@ -9094,7 +9094,7 @@
       <c r="Q22" s="29"/>
       <c r="R22" s="31"/>
       <c r="S22" s="39"/>
-      <c r="T22" s="106"/>
+      <c r="T22" s="93"/>
       <c r="U22" s="44"/>
       <c r="V22" s="44"/>
       <c r="W22" s="45"/>
@@ -9114,7 +9114,7 @@
       <c r="AK22" s="31"/>
     </row>
     <row r="23" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="106"/>
+      <c r="A23" s="93"/>
       <c r="B23" s="55"/>
       <c r="C23" s="44"/>
       <c r="D23" s="45"/>
@@ -9133,7 +9133,7 @@
       <c r="Q23" s="29"/>
       <c r="R23" s="31"/>
       <c r="S23" s="39"/>
-      <c r="T23" s="106"/>
+      <c r="T23" s="93"/>
       <c r="U23" s="32"/>
       <c r="V23" s="1"/>
       <c r="W23" s="2"/>
@@ -9153,7 +9153,7 @@
       <c r="AK23" s="31"/>
     </row>
     <row r="24" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="106"/>
+      <c r="A24" s="93"/>
       <c r="B24" s="44"/>
       <c r="C24" s="44"/>
       <c r="D24" s="44"/>
@@ -9172,7 +9172,7 @@
       <c r="Q24" s="29"/>
       <c r="R24" s="31"/>
       <c r="S24" s="39"/>
-      <c r="T24" s="106"/>
+      <c r="T24" s="93"/>
       <c r="U24" s="32"/>
       <c r="V24" s="1"/>
       <c r="W24" s="2"/>
@@ -9192,7 +9192,7 @@
       <c r="AK24" s="31"/>
     </row>
     <row r="25" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="106"/>
+      <c r="A25" s="93"/>
       <c r="B25" s="44"/>
       <c r="C25" s="44"/>
       <c r="D25" s="45"/>
@@ -9211,7 +9211,7 @@
       <c r="Q25" s="29"/>
       <c r="R25" s="31"/>
       <c r="S25" s="39"/>
-      <c r="T25" s="106"/>
+      <c r="T25" s="93"/>
       <c r="U25" s="32"/>
       <c r="V25" s="1"/>
       <c r="W25" s="2"/>
@@ -9231,7 +9231,7 @@
       <c r="AK25" s="31"/>
     </row>
     <row r="26" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="106"/>
+      <c r="A26" s="93"/>
       <c r="B26" s="44"/>
       <c r="C26" s="44"/>
       <c r="D26" s="44"/>
@@ -9250,7 +9250,7 @@
       <c r="Q26" s="29"/>
       <c r="R26" s="31"/>
       <c r="S26" s="39"/>
-      <c r="T26" s="106"/>
+      <c r="T26" s="93"/>
       <c r="U26" s="32"/>
       <c r="V26" s="1"/>
       <c r="W26" s="2"/>
@@ -9270,7 +9270,7 @@
       <c r="AK26" s="31"/>
     </row>
     <row r="27" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="106"/>
+      <c r="A27" s="93"/>
       <c r="B27" s="44"/>
       <c r="C27" s="44"/>
       <c r="D27" s="44"/>
@@ -9289,7 +9289,7 @@
       <c r="Q27" s="29"/>
       <c r="R27" s="31"/>
       <c r="S27" s="39"/>
-      <c r="T27" s="106"/>
+      <c r="T27" s="93"/>
       <c r="U27" s="32"/>
       <c r="V27" s="1"/>
       <c r="W27" s="2"/>
@@ -9309,7 +9309,7 @@
       <c r="AK27" s="31"/>
     </row>
     <row r="28" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="106"/>
+      <c r="A28" s="93"/>
       <c r="B28" s="44"/>
       <c r="C28" s="44"/>
       <c r="D28" s="44"/>
@@ -9328,7 +9328,7 @@
       <c r="Q28" s="29"/>
       <c r="R28" s="31"/>
       <c r="S28" s="39"/>
-      <c r="T28" s="106"/>
+      <c r="T28" s="93"/>
       <c r="U28" s="32"/>
       <c r="V28" s="1"/>
       <c r="W28" s="2"/>
@@ -9348,7 +9348,7 @@
       <c r="AK28" s="31"/>
     </row>
     <row r="29" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="106"/>
+      <c r="A29" s="93"/>
       <c r="B29" s="44"/>
       <c r="C29" s="44"/>
       <c r="D29" s="44"/>
@@ -9367,7 +9367,7 @@
       <c r="Q29" s="29"/>
       <c r="R29" s="31"/>
       <c r="S29" s="39"/>
-      <c r="T29" s="106"/>
+      <c r="T29" s="93"/>
       <c r="U29" s="32"/>
       <c r="V29" s="1"/>
       <c r="W29" s="2"/>
@@ -9387,7 +9387,7 @@
       <c r="AK29" s="31"/>
     </row>
     <row r="30" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="106"/>
+      <c r="A30" s="93"/>
       <c r="B30" s="44"/>
       <c r="C30" s="44"/>
       <c r="D30" s="44"/>
@@ -9406,7 +9406,7 @@
       <c r="Q30" s="29"/>
       <c r="R30" s="31"/>
       <c r="S30" s="39"/>
-      <c r="T30" s="106"/>
+      <c r="T30" s="93"/>
       <c r="U30" s="32"/>
       <c r="V30" s="1"/>
       <c r="W30" s="2"/>
@@ -9426,7 +9426,7 @@
       <c r="AK30" s="31"/>
     </row>
     <row r="31" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="106"/>
+      <c r="A31" s="93"/>
       <c r="B31" s="44"/>
       <c r="C31" s="44"/>
       <c r="D31" s="44"/>
@@ -9445,7 +9445,7 @@
       <c r="Q31" s="29"/>
       <c r="R31" s="31"/>
       <c r="S31" s="39"/>
-      <c r="T31" s="106"/>
+      <c r="T31" s="93"/>
       <c r="U31" s="32"/>
       <c r="V31" s="1"/>
       <c r="W31" s="2"/>
@@ -9465,7 +9465,7 @@
       <c r="AK31" s="31"/>
     </row>
     <row r="32" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="106"/>
+      <c r="A32" s="93"/>
       <c r="B32" s="44"/>
       <c r="C32" s="44"/>
       <c r="D32" s="44"/>
@@ -9484,7 +9484,7 @@
       <c r="Q32" s="29"/>
       <c r="R32" s="31"/>
       <c r="S32" s="39"/>
-      <c r="T32" s="106"/>
+      <c r="T32" s="93"/>
       <c r="U32" s="32"/>
       <c r="V32" s="1"/>
       <c r="W32" s="2"/>
@@ -9504,7 +9504,7 @@
       <c r="AK32" s="31"/>
     </row>
     <row r="33" spans="1:60" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="106"/>
+      <c r="A33" s="93"/>
       <c r="B33" s="44"/>
       <c r="C33" s="44"/>
       <c r="D33" s="44"/>
@@ -9523,7 +9523,7 @@
       <c r="Q33" s="29"/>
       <c r="R33" s="31"/>
       <c r="S33" s="39"/>
-      <c r="T33" s="106"/>
+      <c r="T33" s="93"/>
       <c r="U33" s="32"/>
       <c r="V33" s="1"/>
       <c r="W33" s="2"/>
@@ -9543,7 +9543,7 @@
       <c r="AK33" s="31"/>
     </row>
     <row r="34" spans="1:60" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="106"/>
+      <c r="A34" s="93"/>
       <c r="B34" s="44"/>
       <c r="C34" s="44"/>
       <c r="D34" s="44"/>
@@ -9562,7 +9562,7 @@
       <c r="Q34" s="29"/>
       <c r="R34" s="31"/>
       <c r="S34" s="39"/>
-      <c r="T34" s="106"/>
+      <c r="T34" s="93"/>
       <c r="U34" s="32"/>
       <c r="V34" s="1"/>
       <c r="W34" s="2"/>
@@ -9582,7 +9582,7 @@
       <c r="AK34" s="31"/>
     </row>
     <row r="35" spans="1:60" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="106"/>
+      <c r="A35" s="93"/>
       <c r="B35" s="44"/>
       <c r="C35" s="44"/>
       <c r="D35" s="44"/>
@@ -9601,7 +9601,7 @@
       <c r="Q35" s="29"/>
       <c r="R35" s="31"/>
       <c r="S35" s="39"/>
-      <c r="T35" s="106"/>
+      <c r="T35" s="93"/>
       <c r="U35" s="32"/>
       <c r="V35" s="1"/>
       <c r="W35" s="2"/>
@@ -9621,7 +9621,7 @@
       <c r="AK35" s="31"/>
     </row>
     <row r="36" spans="1:60" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="106"/>
+      <c r="A36" s="93"/>
       <c r="B36" s="44"/>
       <c r="C36" s="44"/>
       <c r="D36" s="44"/>
@@ -9640,7 +9640,7 @@
       <c r="Q36" s="29"/>
       <c r="R36" s="31"/>
       <c r="S36" s="39"/>
-      <c r="T36" s="106"/>
+      <c r="T36" s="93"/>
       <c r="U36" s="32"/>
       <c r="V36" s="1"/>
       <c r="W36" s="2"/>
@@ -9660,7 +9660,7 @@
       <c r="AK36" s="31"/>
     </row>
     <row r="37" spans="1:60" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="106"/>
+      <c r="A37" s="93"/>
       <c r="B37" s="44"/>
       <c r="C37" s="44"/>
       <c r="D37" s="45"/>
@@ -9679,7 +9679,7 @@
       <c r="Q37" s="29"/>
       <c r="R37" s="31"/>
       <c r="S37" s="39"/>
-      <c r="T37" s="106"/>
+      <c r="T37" s="93"/>
       <c r="U37" s="32"/>
       <c r="V37" s="1"/>
       <c r="W37" s="2"/>
@@ -9699,7 +9699,7 @@
       <c r="AK37" s="31"/>
     </row>
     <row r="38" spans="1:60" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="106"/>
+      <c r="A38" s="93"/>
       <c r="B38" s="54"/>
       <c r="C38" s="52"/>
       <c r="D38" s="52"/>
@@ -9718,7 +9718,7 @@
       <c r="Q38" s="29"/>
       <c r="R38" s="31"/>
       <c r="S38" s="39"/>
-      <c r="T38" s="106"/>
+      <c r="T38" s="93"/>
       <c r="U38" s="32"/>
       <c r="V38" s="1"/>
       <c r="W38" s="2"/>
@@ -9738,7 +9738,7 @@
       <c r="AK38" s="31"/>
     </row>
     <row r="39" spans="1:60" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="106"/>
+      <c r="A39" s="93"/>
       <c r="B39" s="54"/>
       <c r="C39" s="49"/>
       <c r="D39" s="49"/>
@@ -9757,7 +9757,7 @@
       <c r="Q39" s="29"/>
       <c r="R39" s="31"/>
       <c r="S39" s="39"/>
-      <c r="T39" s="106"/>
+      <c r="T39" s="93"/>
       <c r="U39" s="32"/>
       <c r="V39" s="1"/>
       <c r="W39" s="2"/>
@@ -9777,7 +9777,7 @@
       <c r="AK39" s="31"/>
     </row>
     <row r="40" spans="1:60" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="106"/>
+      <c r="A40" s="93"/>
       <c r="B40" s="55"/>
       <c r="C40" s="44"/>
       <c r="D40" s="45"/>
@@ -9796,7 +9796,7 @@
       <c r="Q40" s="29"/>
       <c r="R40" s="31"/>
       <c r="S40" s="39"/>
-      <c r="T40" s="106"/>
+      <c r="T40" s="93"/>
       <c r="U40" s="32"/>
       <c r="V40" s="1"/>
       <c r="W40" s="2"/>
@@ -9816,7 +9816,7 @@
       <c r="AK40" s="31"/>
     </row>
     <row r="41" spans="1:60" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="107"/>
+      <c r="A41" s="94"/>
       <c r="B41" s="44"/>
       <c r="C41" s="44"/>
       <c r="D41" s="44"/>
@@ -9835,7 +9835,7 @@
       <c r="Q41" s="29"/>
       <c r="R41" s="31"/>
       <c r="S41" s="40"/>
-      <c r="T41" s="107"/>
+      <c r="T41" s="94"/>
       <c r="U41" s="32"/>
       <c r="V41" s="1"/>
       <c r="W41" s="2"/>
@@ -9881,21 +9881,21 @@
       <c r="C43" s="15"/>
       <c r="D43" s="16"/>
       <c r="E43" s="14"/>
-      <c r="F43" s="85" t="s">
+      <c r="F43" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="G43" s="85"/>
-      <c r="H43" s="85"/>
-      <c r="I43" s="86" t="s">
+      <c r="G43" s="89"/>
+      <c r="H43" s="89"/>
+      <c r="I43" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="J43" s="86"/>
-      <c r="K43" s="86"/>
-      <c r="L43" s="87" t="s">
+      <c r="J43" s="90"/>
+      <c r="K43" s="90"/>
+      <c r="L43" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="M43" s="87"/>
-      <c r="N43" s="87"/>
+      <c r="M43" s="91"/>
+      <c r="N43" s="91"/>
       <c r="O43" s="88" t="s">
         <v>19</v>
       </c>
@@ -9908,21 +9908,21 @@
       <c r="V43" s="23"/>
       <c r="W43" s="23"/>
       <c r="X43" s="23"/>
-      <c r="Y43" s="85" t="s">
+      <c r="Y43" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="Z43" s="85"/>
-      <c r="AA43" s="85"/>
-      <c r="AB43" s="86" t="s">
+      <c r="Z43" s="89"/>
+      <c r="AA43" s="89"/>
+      <c r="AB43" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="AC43" s="86"/>
-      <c r="AD43" s="86"/>
-      <c r="AE43" s="87" t="s">
+      <c r="AC43" s="90"/>
+      <c r="AD43" s="90"/>
+      <c r="AE43" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="AF43" s="87"/>
-      <c r="AG43" s="87"/>
+      <c r="AF43" s="91"/>
+      <c r="AG43" s="91"/>
       <c r="AH43" s="88" t="s">
         <v>19</v>
       </c>
@@ -9954,49 +9954,49 @@
       <c r="BH43" s="17"/>
     </row>
     <row r="44" spans="1:60" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F44" s="89" t="s">
+      <c r="F44" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="G44" s="90"/>
-      <c r="H44" s="91"/>
-      <c r="I44" s="89" t="s">
+      <c r="G44" s="86"/>
+      <c r="H44" s="87"/>
+      <c r="I44" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="J44" s="90"/>
-      <c r="K44" s="91"/>
-      <c r="L44" s="89" t="s">
+      <c r="J44" s="86"/>
+      <c r="K44" s="87"/>
+      <c r="L44" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="M44" s="90"/>
-      <c r="N44" s="91"/>
-      <c r="O44" s="89" t="s">
+      <c r="M44" s="86"/>
+      <c r="N44" s="87"/>
+      <c r="O44" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="P44" s="90"/>
-      <c r="Q44" s="91"/>
+      <c r="P44" s="86"/>
+      <c r="Q44" s="87"/>
       <c r="R44" s="36"/>
       <c r="S44" s="37"/>
       <c r="U44" s="19"/>
-      <c r="Y44" s="89" t="s">
+      <c r="Y44" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="Z44" s="90"/>
-      <c r="AA44" s="91"/>
-      <c r="AB44" s="89" t="s">
+      <c r="Z44" s="86"/>
+      <c r="AA44" s="87"/>
+      <c r="AB44" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="AC44" s="90"/>
-      <c r="AD44" s="91"/>
-      <c r="AE44" s="89" t="s">
+      <c r="AC44" s="86"/>
+      <c r="AD44" s="87"/>
+      <c r="AE44" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="AF44" s="90"/>
-      <c r="AG44" s="91"/>
-      <c r="AH44" s="89" t="s">
+      <c r="AF44" s="86"/>
+      <c r="AG44" s="87"/>
+      <c r="AH44" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="AI44" s="90"/>
-      <c r="AJ44" s="91"/>
+      <c r="AI44" s="86"/>
+      <c r="AJ44" s="87"/>
       <c r="AK44" s="36"/>
     </row>
     <row r="45" spans="1:60" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10111,7 +10111,7 @@
       </c>
     </row>
     <row r="46" spans="1:60" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="108" t="s">
+      <c r="A46" s="95" t="s">
         <v>4</v>
       </c>
       <c r="B46" s="47">
@@ -10152,7 +10152,7 @@
       <c r="Q46" s="57"/>
       <c r="R46" s="75"/>
       <c r="S46" s="11"/>
-      <c r="T46" s="101" t="s">
+      <c r="T46" s="103" t="s">
         <v>4</v>
       </c>
       <c r="U46" s="76"/>
@@ -10174,7 +10174,7 @@
       <c r="AK46" s="75"/>
     </row>
     <row r="47" spans="1:60" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="109"/>
+      <c r="A47" s="96"/>
       <c r="B47" s="47">
         <v>7096314</v>
       </c>
@@ -10213,7 +10213,7 @@
       <c r="Q47" s="57"/>
       <c r="R47" s="75"/>
       <c r="S47" s="12"/>
-      <c r="T47" s="102"/>
+      <c r="T47" s="104"/>
       <c r="U47" s="44"/>
       <c r="V47" s="44"/>
       <c r="W47" s="45"/>
@@ -10233,7 +10233,7 @@
       <c r="AK47" s="31"/>
     </row>
     <row r="48" spans="1:60" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="109"/>
+      <c r="A48" s="96"/>
       <c r="B48" s="81">
         <v>7093513</v>
       </c>
@@ -10272,7 +10272,7 @@
       <c r="Q48" s="57"/>
       <c r="R48" s="75"/>
       <c r="S48" s="41"/>
-      <c r="T48" s="102"/>
+      <c r="T48" s="104"/>
       <c r="U48" s="55"/>
       <c r="V48" s="44"/>
       <c r="W48" s="45"/>
@@ -10292,7 +10292,7 @@
       <c r="AK48" s="31"/>
     </row>
     <row r="49" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="109"/>
+      <c r="A49" s="96"/>
       <c r="B49" s="53">
         <v>7092642</v>
       </c>
@@ -10318,7 +10318,7 @@
         <v>61</v>
       </c>
       <c r="L49" s="57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M49" s="57" t="s">
         <v>60</v>
@@ -10331,7 +10331,7 @@
       <c r="Q49" s="57"/>
       <c r="R49" s="75"/>
       <c r="S49" s="41"/>
-      <c r="T49" s="102"/>
+      <c r="T49" s="104"/>
       <c r="U49" s="54"/>
       <c r="V49" s="52"/>
       <c r="W49" s="52"/>
@@ -10351,7 +10351,7 @@
       <c r="AK49" s="31"/>
     </row>
     <row r="50" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="109"/>
+      <c r="A50" s="96"/>
       <c r="B50" s="53">
         <v>7096839</v>
       </c>
@@ -10378,7 +10378,7 @@
       <c r="Q50" s="57"/>
       <c r="R50" s="75"/>
       <c r="S50" s="41"/>
-      <c r="T50" s="102"/>
+      <c r="T50" s="104"/>
       <c r="U50" s="54"/>
       <c r="V50" s="52"/>
       <c r="W50" s="52"/>
@@ -10398,7 +10398,7 @@
       <c r="AK50" s="31"/>
     </row>
     <row r="51" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="109"/>
+      <c r="A51" s="96"/>
       <c r="B51" s="53">
         <v>7401072</v>
       </c>
@@ -10425,7 +10425,7 @@
       <c r="Q51" s="57"/>
       <c r="R51" s="75"/>
       <c r="S51" s="41"/>
-      <c r="T51" s="102"/>
+      <c r="T51" s="104"/>
       <c r="U51" s="44"/>
       <c r="V51" s="44"/>
       <c r="W51" s="45"/>
@@ -10445,7 +10445,7 @@
       <c r="AK51" s="31"/>
     </row>
     <row r="52" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="109"/>
+      <c r="A52" s="96"/>
       <c r="B52" s="53">
         <v>7077343</v>
       </c>
@@ -10472,7 +10472,7 @@
       <c r="Q52" s="57"/>
       <c r="R52" s="75"/>
       <c r="S52" s="41"/>
-      <c r="T52" s="102"/>
+      <c r="T52" s="104"/>
       <c r="U52" s="44"/>
       <c r="V52" s="44"/>
       <c r="W52" s="45"/>
@@ -10492,7 +10492,7 @@
       <c r="AK52" s="31"/>
     </row>
     <row r="53" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="109"/>
+      <c r="A53" s="96"/>
       <c r="B53" s="53">
         <v>7029156</v>
       </c>
@@ -10519,7 +10519,7 @@
       <c r="Q53" s="57"/>
       <c r="R53" s="75"/>
       <c r="S53" s="41"/>
-      <c r="T53" s="102"/>
+      <c r="T53" s="104"/>
       <c r="U53" s="55"/>
       <c r="V53" s="44"/>
       <c r="W53" s="45"/>
@@ -10539,7 +10539,7 @@
       <c r="AK53" s="31"/>
     </row>
     <row r="54" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="109"/>
+      <c r="A54" s="96"/>
       <c r="B54" s="53">
         <v>7401131</v>
       </c>
@@ -10566,7 +10566,7 @@
       <c r="Q54" s="57"/>
       <c r="R54" s="75"/>
       <c r="S54" s="41"/>
-      <c r="T54" s="102"/>
+      <c r="T54" s="104"/>
       <c r="U54" s="44"/>
       <c r="V54" s="44"/>
       <c r="W54" s="45"/>
@@ -10586,7 +10586,7 @@
       <c r="AK54" s="31"/>
     </row>
     <row r="55" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="109"/>
+      <c r="A55" s="96"/>
       <c r="B55" s="81">
         <v>7051920</v>
       </c>
@@ -10613,7 +10613,7 @@
       <c r="Q55" s="57"/>
       <c r="R55" s="75"/>
       <c r="S55" s="41"/>
-      <c r="T55" s="102"/>
+      <c r="T55" s="104"/>
       <c r="U55" s="44"/>
       <c r="V55" s="44"/>
       <c r="W55" s="45"/>
@@ -10633,7 +10633,7 @@
       <c r="AK55" s="31"/>
     </row>
     <row r="56" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="109"/>
+      <c r="A56" s="96"/>
       <c r="B56" s="53">
         <v>7092738</v>
       </c>
@@ -10660,7 +10660,7 @@
       <c r="Q56" s="57"/>
       <c r="R56" s="75"/>
       <c r="S56" s="41"/>
-      <c r="T56" s="102"/>
+      <c r="T56" s="104"/>
       <c r="U56" s="44"/>
       <c r="V56" s="44"/>
       <c r="W56" s="45"/>
@@ -10680,7 +10680,7 @@
       <c r="AK56" s="31"/>
     </row>
     <row r="57" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="109"/>
+      <c r="A57" s="96"/>
       <c r="B57" s="53">
         <v>7045037</v>
       </c>
@@ -10707,7 +10707,7 @@
       <c r="Q57" s="57"/>
       <c r="R57" s="75"/>
       <c r="S57" s="41"/>
-      <c r="T57" s="102"/>
+      <c r="T57" s="104"/>
       <c r="U57" s="55"/>
       <c r="V57" s="44"/>
       <c r="W57" s="45"/>
@@ -10727,7 +10727,7 @@
       <c r="AK57" s="31"/>
     </row>
     <row r="58" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="109"/>
+      <c r="A58" s="96"/>
       <c r="B58" s="53">
         <v>7401055</v>
       </c>
@@ -10754,7 +10754,7 @@
       <c r="Q58" s="57"/>
       <c r="R58" s="75"/>
       <c r="S58" s="41"/>
-      <c r="T58" s="102"/>
+      <c r="T58" s="104"/>
       <c r="U58" s="44"/>
       <c r="V58" s="44"/>
       <c r="W58" s="45"/>
@@ -10774,7 +10774,7 @@
       <c r="AK58" s="31"/>
     </row>
     <row r="59" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="109"/>
+      <c r="A59" s="96"/>
       <c r="B59" s="44"/>
       <c r="C59" s="44"/>
       <c r="D59" s="45"/>
@@ -10793,7 +10793,7 @@
       <c r="Q59" s="29"/>
       <c r="R59" s="31"/>
       <c r="S59" s="41"/>
-      <c r="T59" s="102"/>
+      <c r="T59" s="104"/>
       <c r="U59" s="44"/>
       <c r="V59" s="44"/>
       <c r="W59" s="45"/>
@@ -10813,7 +10813,7 @@
       <c r="AK59" s="31"/>
     </row>
     <row r="60" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="109"/>
+      <c r="A60" s="96"/>
       <c r="B60" s="44"/>
       <c r="C60" s="44"/>
       <c r="D60" s="45"/>
@@ -10832,7 +10832,7 @@
       <c r="Q60" s="29"/>
       <c r="R60" s="31"/>
       <c r="S60" s="41"/>
-      <c r="T60" s="102"/>
+      <c r="T60" s="104"/>
       <c r="U60" s="44"/>
       <c r="V60" s="44"/>
       <c r="W60" s="45"/>
@@ -10852,7 +10852,7 @@
       <c r="AK60" s="31"/>
     </row>
     <row r="61" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="109"/>
+      <c r="A61" s="96"/>
       <c r="B61" s="44"/>
       <c r="C61" s="44"/>
       <c r="D61" s="45"/>
@@ -10871,7 +10871,7 @@
       <c r="Q61" s="29"/>
       <c r="R61" s="31"/>
       <c r="S61" s="41"/>
-      <c r="T61" s="102"/>
+      <c r="T61" s="104"/>
       <c r="U61" s="55"/>
       <c r="V61" s="44"/>
       <c r="W61" s="45"/>
@@ -10891,7 +10891,7 @@
       <c r="AK61" s="31"/>
     </row>
     <row r="62" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="109"/>
+      <c r="A62" s="96"/>
       <c r="B62" s="54"/>
       <c r="C62" s="49"/>
       <c r="D62" s="49"/>
@@ -10910,7 +10910,7 @@
       <c r="Q62" s="29"/>
       <c r="R62" s="31"/>
       <c r="S62" s="41"/>
-      <c r="T62" s="102"/>
+      <c r="T62" s="104"/>
       <c r="U62" s="54"/>
       <c r="V62" s="52"/>
       <c r="W62" s="52"/>
@@ -10930,7 +10930,7 @@
       <c r="AK62" s="31"/>
     </row>
     <row r="63" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="109"/>
+      <c r="A63" s="96"/>
       <c r="B63" s="47"/>
       <c r="C63" s="44"/>
       <c r="D63" s="45"/>
@@ -10949,7 +10949,7 @@
       <c r="Q63" s="29"/>
       <c r="R63" s="31"/>
       <c r="S63" s="41"/>
-      <c r="T63" s="102"/>
+      <c r="T63" s="104"/>
       <c r="U63" s="54"/>
       <c r="V63" s="52"/>
       <c r="W63" s="52"/>
@@ -10969,7 +10969,7 @@
       <c r="AK63" s="31"/>
     </row>
     <row r="64" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="109"/>
+      <c r="A64" s="96"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -10988,7 +10988,7 @@
       <c r="Q64" s="29"/>
       <c r="R64" s="31"/>
       <c r="S64" s="41"/>
-      <c r="T64" s="102"/>
+      <c r="T64" s="104"/>
       <c r="U64" s="47"/>
       <c r="V64" s="47"/>
       <c r="W64" s="47"/>
@@ -11008,7 +11008,7 @@
       <c r="AK64" s="31"/>
     </row>
     <row r="65" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="109"/>
+      <c r="A65" s="96"/>
       <c r="B65" s="44"/>
       <c r="C65" s="44"/>
       <c r="D65" s="44"/>
@@ -11027,7 +11027,7 @@
       <c r="Q65" s="29"/>
       <c r="R65" s="31"/>
       <c r="S65" s="41"/>
-      <c r="T65" s="102"/>
+      <c r="T65" s="104"/>
       <c r="U65" s="44"/>
       <c r="V65" s="44"/>
       <c r="W65" s="45"/>
@@ -11047,7 +11047,7 @@
       <c r="AK65" s="31"/>
     </row>
     <row r="66" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="109"/>
+      <c r="A66" s="96"/>
       <c r="B66" s="55"/>
       <c r="C66" s="44"/>
       <c r="D66" s="45"/>
@@ -11066,7 +11066,7 @@
       <c r="Q66" s="29"/>
       <c r="R66" s="31"/>
       <c r="S66" s="41"/>
-      <c r="T66" s="102"/>
+      <c r="T66" s="104"/>
       <c r="U66" s="44"/>
       <c r="V66" s="44"/>
       <c r="W66" s="45"/>
@@ -11086,7 +11086,7 @@
       <c r="AK66" s="31"/>
     </row>
     <row r="67" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="109"/>
+      <c r="A67" s="96"/>
       <c r="B67" s="44"/>
       <c r="C67" s="44"/>
       <c r="D67" s="45"/>
@@ -11105,7 +11105,7 @@
       <c r="Q67" s="29"/>
       <c r="R67" s="31"/>
       <c r="S67" s="41"/>
-      <c r="T67" s="102"/>
+      <c r="T67" s="104"/>
       <c r="U67" s="55"/>
       <c r="V67" s="44"/>
       <c r="W67" s="45"/>
@@ -11125,7 +11125,7 @@
       <c r="AK67" s="31"/>
     </row>
     <row r="68" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="109"/>
+      <c r="A68" s="96"/>
       <c r="B68" s="47"/>
       <c r="C68" s="44"/>
       <c r="D68" s="45"/>
@@ -11144,7 +11144,7 @@
       <c r="Q68" s="29"/>
       <c r="R68" s="31"/>
       <c r="S68" s="41"/>
-      <c r="T68" s="102"/>
+      <c r="T68" s="104"/>
       <c r="U68" s="1"/>
       <c r="V68" s="1"/>
       <c r="W68" s="2"/>
@@ -11164,7 +11164,7 @@
       <c r="AK68" s="31"/>
     </row>
     <row r="69" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="109"/>
+      <c r="A69" s="96"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -11183,7 +11183,7 @@
       <c r="Q69" s="29"/>
       <c r="R69" s="31"/>
       <c r="S69" s="41"/>
-      <c r="T69" s="102"/>
+      <c r="T69" s="104"/>
       <c r="U69" s="1"/>
       <c r="V69" s="1"/>
       <c r="W69" s="2"/>
@@ -11203,7 +11203,7 @@
       <c r="AK69" s="31"/>
     </row>
     <row r="70" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="109"/>
+      <c r="A70" s="96"/>
       <c r="B70" s="54"/>
       <c r="C70" s="56"/>
       <c r="D70" s="56"/>
@@ -11222,7 +11222,7 @@
       <c r="Q70" s="29"/>
       <c r="R70" s="31"/>
       <c r="S70" s="41"/>
-      <c r="T70" s="102"/>
+      <c r="T70" s="104"/>
       <c r="U70" s="1"/>
       <c r="V70" s="1"/>
       <c r="W70" s="2"/>
@@ -11242,7 +11242,7 @@
       <c r="AK70" s="31"/>
     </row>
     <row r="71" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="109"/>
+      <c r="A71" s="96"/>
       <c r="B71" s="48"/>
       <c r="C71" s="49"/>
       <c r="D71" s="49"/>
@@ -11261,7 +11261,7 @@
       <c r="Q71" s="29"/>
       <c r="R71" s="31"/>
       <c r="S71" s="41"/>
-      <c r="T71" s="102"/>
+      <c r="T71" s="104"/>
       <c r="U71" s="1"/>
       <c r="V71" s="1"/>
       <c r="W71" s="2"/>
@@ -11281,7 +11281,7 @@
       <c r="AK71" s="31"/>
     </row>
     <row r="72" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="109"/>
+      <c r="A72" s="96"/>
       <c r="B72" s="47"/>
       <c r="C72" s="44"/>
       <c r="D72" s="45"/>
@@ -11300,7 +11300,7 @@
       <c r="Q72" s="29"/>
       <c r="R72" s="31"/>
       <c r="S72" s="41"/>
-      <c r="T72" s="102"/>
+      <c r="T72" s="104"/>
       <c r="U72" s="1"/>
       <c r="V72" s="1"/>
       <c r="W72" s="2"/>
@@ -11320,7 +11320,7 @@
       <c r="AK72" s="31"/>
     </row>
     <row r="73" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="109"/>
+      <c r="A73" s="96"/>
       <c r="B73" s="48"/>
       <c r="C73" s="49"/>
       <c r="D73" s="49"/>
@@ -11339,7 +11339,7 @@
       <c r="Q73" s="29"/>
       <c r="R73" s="31"/>
       <c r="S73" s="41"/>
-      <c r="T73" s="102"/>
+      <c r="T73" s="104"/>
       <c r="U73" s="1"/>
       <c r="V73" s="1"/>
       <c r="W73" s="2"/>
@@ -11357,7 +11357,7 @@
       <c r="AK73" s="31"/>
     </row>
     <row r="74" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="109"/>
+      <c r="A74" s="96"/>
       <c r="B74" s="47"/>
       <c r="C74" s="44"/>
       <c r="D74" s="45"/>
@@ -11376,7 +11376,7 @@
       <c r="Q74" s="29"/>
       <c r="R74" s="31"/>
       <c r="S74" s="41"/>
-      <c r="T74" s="102"/>
+      <c r="T74" s="104"/>
       <c r="U74" s="1"/>
       <c r="V74" s="1"/>
       <c r="W74" s="2"/>
@@ -11394,7 +11394,7 @@
       <c r="AK74" s="31"/>
     </row>
     <row r="75" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="109"/>
+      <c r="A75" s="96"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -11413,7 +11413,7 @@
       <c r="Q75" s="29"/>
       <c r="R75" s="31"/>
       <c r="S75" s="41"/>
-      <c r="T75" s="102"/>
+      <c r="T75" s="104"/>
       <c r="U75" s="1"/>
       <c r="V75" s="1"/>
       <c r="W75" s="2"/>
@@ -11431,7 +11431,7 @@
       <c r="AK75" s="31"/>
     </row>
     <row r="76" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="109"/>
+      <c r="A76" s="96"/>
       <c r="B76" s="47"/>
       <c r="C76" s="44"/>
       <c r="D76" s="45"/>
@@ -11450,7 +11450,7 @@
       <c r="Q76" s="29"/>
       <c r="R76" s="31"/>
       <c r="S76" s="41"/>
-      <c r="T76" s="102"/>
+      <c r="T76" s="104"/>
       <c r="U76" s="1"/>
       <c r="V76" s="1"/>
       <c r="W76" s="2"/>
@@ -11468,7 +11468,7 @@
       <c r="AK76" s="31"/>
     </row>
     <row r="77" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="109"/>
+      <c r="A77" s="96"/>
       <c r="B77" s="55"/>
       <c r="C77" s="44"/>
       <c r="D77" s="45"/>
@@ -11487,7 +11487,7 @@
       <c r="Q77" s="29"/>
       <c r="R77" s="31"/>
       <c r="S77" s="41"/>
-      <c r="T77" s="102"/>
+      <c r="T77" s="104"/>
       <c r="U77" s="1"/>
       <c r="V77" s="1"/>
       <c r="W77" s="2"/>
@@ -11505,7 +11505,7 @@
       <c r="AK77" s="31"/>
     </row>
     <row r="78" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="109"/>
+      <c r="A78" s="96"/>
       <c r="B78" s="54"/>
       <c r="C78" s="49"/>
       <c r="D78" s="49"/>
@@ -11524,7 +11524,7 @@
       <c r="Q78" s="29"/>
       <c r="R78" s="31"/>
       <c r="S78" s="41"/>
-      <c r="T78" s="102"/>
+      <c r="T78" s="104"/>
       <c r="U78" s="1"/>
       <c r="V78" s="1"/>
       <c r="W78" s="2"/>
@@ -11542,7 +11542,7 @@
       <c r="AK78" s="31"/>
     </row>
     <row r="79" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="109"/>
+      <c r="A79" s="96"/>
       <c r="B79" s="44"/>
       <c r="C79" s="44"/>
       <c r="D79" s="45"/>
@@ -11561,7 +11561,7 @@
       <c r="Q79" s="29"/>
       <c r="R79" s="31"/>
       <c r="S79" s="41"/>
-      <c r="T79" s="102"/>
+      <c r="T79" s="104"/>
       <c r="U79" s="1"/>
       <c r="V79" s="1"/>
       <c r="W79" s="2"/>
@@ -11579,7 +11579,7 @@
       <c r="AK79" s="31"/>
     </row>
     <row r="80" spans="1:37" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="109"/>
+      <c r="A80" s="96"/>
       <c r="B80" s="44"/>
       <c r="C80" s="44"/>
       <c r="D80" s="45"/>
@@ -11598,7 +11598,7 @@
       <c r="Q80" s="29"/>
       <c r="R80" s="31"/>
       <c r="S80" s="41"/>
-      <c r="T80" s="102"/>
+      <c r="T80" s="104"/>
       <c r="U80" s="1"/>
       <c r="V80" s="1"/>
       <c r="W80" s="2"/>
@@ -11616,7 +11616,7 @@
       <c r="AK80" s="31"/>
     </row>
     <row r="81" spans="1:60" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="109"/>
+      <c r="A81" s="96"/>
       <c r="B81" s="44"/>
       <c r="C81" s="44"/>
       <c r="D81" s="45"/>
@@ -11635,7 +11635,7 @@
       <c r="Q81" s="29"/>
       <c r="R81" s="31"/>
       <c r="S81" s="41"/>
-      <c r="T81" s="102"/>
+      <c r="T81" s="104"/>
       <c r="U81" s="1"/>
       <c r="V81" s="1"/>
       <c r="W81" s="2"/>
@@ -11653,7 +11653,7 @@
       <c r="AK81" s="31"/>
     </row>
     <row r="82" spans="1:60" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="110"/>
+      <c r="A82" s="97"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="2"/>
@@ -11672,7 +11672,7 @@
       <c r="Q82" s="29"/>
       <c r="R82" s="31"/>
       <c r="S82" s="41"/>
-      <c r="T82" s="103"/>
+      <c r="T82" s="105"/>
       <c r="U82" s="1"/>
       <c r="V82" s="1"/>
       <c r="W82" s="2"/>
@@ -11736,21 +11736,21 @@
       <c r="V84" s="23"/>
       <c r="W84" s="23"/>
       <c r="X84" s="23"/>
-      <c r="Y84" s="85" t="s">
+      <c r="Y84" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="Z84" s="85"/>
-      <c r="AA84" s="85"/>
-      <c r="AB84" s="86" t="s">
+      <c r="Z84" s="89"/>
+      <c r="AA84" s="89"/>
+      <c r="AB84" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="AC84" s="86"/>
-      <c r="AD84" s="86"/>
-      <c r="AE84" s="87" t="s">
+      <c r="AC84" s="90"/>
+      <c r="AD84" s="90"/>
+      <c r="AE84" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="AF84" s="87"/>
-      <c r="AG84" s="87"/>
+      <c r="AF84" s="91"/>
+      <c r="AG84" s="91"/>
       <c r="AH84" s="88" t="s">
         <v>19</v>
       </c>
@@ -11787,21 +11787,21 @@
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
       <c r="E85" s="14"/>
-      <c r="F85" s="85" t="s">
+      <c r="F85" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="G85" s="85"/>
-      <c r="H85" s="85"/>
-      <c r="I85" s="86" t="s">
+      <c r="G85" s="89"/>
+      <c r="H85" s="89"/>
+      <c r="I85" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="J85" s="86"/>
-      <c r="K85" s="86"/>
-      <c r="L85" s="87" t="s">
+      <c r="J85" s="90"/>
+      <c r="K85" s="90"/>
+      <c r="L85" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="M85" s="87"/>
-      <c r="N85" s="87"/>
+      <c r="M85" s="91"/>
+      <c r="N85" s="91"/>
       <c r="O85" s="88" t="s">
         <v>19</v>
       </c>
@@ -11810,26 +11810,26 @@
       <c r="R85" s="36"/>
       <c r="S85" s="37"/>
       <c r="U85" s="19"/>
-      <c r="Y85" s="89" t="s">
+      <c r="Y85" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="Z85" s="90"/>
-      <c r="AA85" s="91"/>
-      <c r="AB85" s="89" t="s">
+      <c r="Z85" s="86"/>
+      <c r="AA85" s="87"/>
+      <c r="AB85" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="AC85" s="90"/>
-      <c r="AD85" s="91"/>
-      <c r="AE85" s="89" t="s">
+      <c r="AC85" s="86"/>
+      <c r="AD85" s="87"/>
+      <c r="AE85" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="AF85" s="90"/>
-      <c r="AG85" s="91"/>
-      <c r="AH85" s="89" t="s">
+      <c r="AF85" s="86"/>
+      <c r="AG85" s="87"/>
+      <c r="AH85" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="AI85" s="90"/>
-      <c r="AJ85" s="91"/>
+      <c r="AI85" s="86"/>
+      <c r="AJ85" s="87"/>
       <c r="AK85" s="36"/>
     </row>
     <row r="86" spans="1:60" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -11839,26 +11839,26 @@
       <c r="B86" s="21"/>
       <c r="C86" s="21"/>
       <c r="D86" s="21"/>
-      <c r="F86" s="89" t="s">
+      <c r="F86" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="G86" s="90"/>
-      <c r="H86" s="91"/>
-      <c r="I86" s="89" t="s">
+      <c r="G86" s="86"/>
+      <c r="H86" s="87"/>
+      <c r="I86" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="J86" s="90"/>
-      <c r="K86" s="91"/>
-      <c r="L86" s="89" t="s">
+      <c r="J86" s="86"/>
+      <c r="K86" s="87"/>
+      <c r="L86" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="M86" s="90"/>
-      <c r="N86" s="91"/>
-      <c r="O86" s="89" t="s">
+      <c r="M86" s="86"/>
+      <c r="N86" s="87"/>
+      <c r="O86" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="P86" s="90"/>
-      <c r="Q86" s="91"/>
+      <c r="P86" s="86"/>
+      <c r="Q86" s="87"/>
       <c r="R86" s="36"/>
       <c r="S86" s="38"/>
       <c r="T86" s="18" t="s">
@@ -11917,7 +11917,7 @@
       </c>
     </row>
     <row r="87" spans="1:60" s="17" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="99" t="s">
+      <c r="A87" s="101" t="s">
         <v>3</v>
       </c>
       <c r="B87" s="18" t="s">
@@ -11972,7 +11972,7 @@
         <v>20</v>
       </c>
       <c r="S87" s="42"/>
-      <c r="T87" s="99" t="s">
+      <c r="T87" s="101" t="s">
         <v>3</v>
       </c>
       <c r="U87" s="44"/>
@@ -11994,7 +11994,7 @@
       <c r="AK87" s="79"/>
     </row>
     <row r="88" spans="1:60" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="100"/>
+      <c r="A88" s="102"/>
       <c r="B88" s="44"/>
       <c r="C88" s="44"/>
       <c r="D88" s="45"/>
@@ -12013,7 +12013,7 @@
       <c r="Q88" s="29"/>
       <c r="R88" s="79"/>
       <c r="S88" s="42"/>
-      <c r="T88" s="100"/>
+      <c r="T88" s="102"/>
       <c r="U88" s="44"/>
       <c r="V88" s="44"/>
       <c r="W88" s="45"/>
@@ -12033,7 +12033,7 @@
       <c r="AK88" s="68"/>
     </row>
     <row r="89" spans="1:60" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="100"/>
+      <c r="A89" s="102"/>
       <c r="B89" s="44"/>
       <c r="C89" s="44"/>
       <c r="D89" s="45"/>
@@ -12052,7 +12052,7 @@
       <c r="Q89" s="29"/>
       <c r="R89" s="68"/>
       <c r="S89" s="42"/>
-      <c r="T89" s="100"/>
+      <c r="T89" s="102"/>
       <c r="U89" s="54"/>
       <c r="V89" s="52"/>
       <c r="W89" s="52"/>
@@ -12072,7 +12072,7 @@
       <c r="AK89" s="68"/>
     </row>
     <row r="90" spans="1:60" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="100"/>
+      <c r="A90" s="102"/>
       <c r="B90" s="53"/>
       <c r="C90" s="53"/>
       <c r="D90" s="65"/>
@@ -12091,7 +12091,7 @@
       <c r="Q90" s="29"/>
       <c r="R90" s="68"/>
       <c r="S90" s="42"/>
-      <c r="T90" s="100"/>
+      <c r="T90" s="102"/>
       <c r="U90" s="44"/>
       <c r="V90" s="44"/>
       <c r="W90" s="45"/>
@@ -12111,7 +12111,7 @@
       <c r="AK90" s="68"/>
     </row>
     <row r="91" spans="1:60" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="100"/>
+      <c r="A91" s="102"/>
       <c r="B91" s="44"/>
       <c r="C91" s="44"/>
       <c r="D91" s="44"/>
@@ -12130,7 +12130,7 @@
       <c r="Q91" s="29"/>
       <c r="R91" s="68"/>
       <c r="S91" s="43"/>
-      <c r="T91" s="100"/>
+      <c r="T91" s="102"/>
       <c r="U91" s="44"/>
       <c r="V91" s="44"/>
       <c r="W91" s="45"/>
@@ -12150,7 +12150,7 @@
       <c r="AK91" s="69"/>
     </row>
     <row r="92" spans="1:60" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="100"/>
+      <c r="A92" s="102"/>
       <c r="B92" s="47"/>
       <c r="C92" s="44"/>
       <c r="D92" s="45"/>
@@ -12169,7 +12169,7 @@
       <c r="Q92" s="29"/>
       <c r="R92" s="69"/>
       <c r="S92" s="42"/>
-      <c r="T92" s="100"/>
+      <c r="T92" s="102"/>
       <c r="U92" s="54"/>
       <c r="V92" s="52"/>
       <c r="W92" s="52"/>
@@ -12189,7 +12189,7 @@
       <c r="AK92" s="68"/>
     </row>
     <row r="93" spans="1:60" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="100"/>
+      <c r="A93" s="102"/>
       <c r="B93" s="54"/>
       <c r="C93" s="52"/>
       <c r="D93" s="52"/>
@@ -12208,7 +12208,7 @@
       <c r="Q93" s="29"/>
       <c r="R93" s="68"/>
       <c r="S93" s="42"/>
-      <c r="T93" s="100"/>
+      <c r="T93" s="102"/>
       <c r="U93" s="44"/>
       <c r="V93" s="44"/>
       <c r="W93" s="45"/>
@@ -12228,7 +12228,7 @@
       <c r="AK93" s="68"/>
     </row>
     <row r="94" spans="1:60" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="100"/>
+      <c r="A94" s="102"/>
       <c r="B94" s="54"/>
       <c r="C94" s="49"/>
       <c r="D94" s="49"/>
@@ -12247,7 +12247,7 @@
       <c r="Q94" s="29"/>
       <c r="R94" s="68"/>
       <c r="S94" s="42"/>
-      <c r="T94" s="100"/>
+      <c r="T94" s="102"/>
       <c r="U94" s="44"/>
       <c r="V94" s="44"/>
       <c r="W94" s="45"/>
@@ -12267,7 +12267,7 @@
       <c r="AK94" s="68"/>
     </row>
     <row r="95" spans="1:60" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="100"/>
+      <c r="A95" s="102"/>
       <c r="B95" s="44"/>
       <c r="C95" s="44"/>
       <c r="D95" s="45"/>
@@ -12286,7 +12286,7 @@
       <c r="Q95" s="29"/>
       <c r="R95" s="68"/>
       <c r="S95" s="42"/>
-      <c r="T95" s="100"/>
+      <c r="T95" s="102"/>
       <c r="U95" s="54"/>
       <c r="V95" s="52"/>
       <c r="W95" s="52"/>
@@ -12306,7 +12306,7 @@
       <c r="AK95" s="68"/>
     </row>
     <row r="96" spans="1:60" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="100"/>
+      <c r="A96" s="102"/>
       <c r="B96" s="55"/>
       <c r="C96" s="44"/>
       <c r="D96" s="45"/>
@@ -12325,7 +12325,7 @@
       <c r="Q96" s="29"/>
       <c r="R96" s="68"/>
       <c r="S96" s="42"/>
-      <c r="T96" s="100"/>
+      <c r="T96" s="102"/>
       <c r="U96" s="54"/>
       <c r="V96" s="52"/>
       <c r="W96" s="52"/>
@@ -12345,7 +12345,7 @@
       <c r="AK96" s="68"/>
     </row>
     <row r="97" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="100"/>
+      <c r="A97" s="102"/>
       <c r="B97" s="44"/>
       <c r="C97" s="44"/>
       <c r="D97" s="45"/>
@@ -12364,7 +12364,7 @@
       <c r="Q97" s="29"/>
       <c r="R97" s="68"/>
       <c r="S97" s="43"/>
-      <c r="T97" s="100"/>
+      <c r="T97" s="102"/>
       <c r="U97" s="47"/>
       <c r="V97" s="44"/>
       <c r="W97" s="45"/>
@@ -12384,7 +12384,7 @@
       <c r="AK97" s="69"/>
     </row>
     <row r="98" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="100"/>
+      <c r="A98" s="102"/>
       <c r="B98" s="44"/>
       <c r="C98" s="44"/>
       <c r="D98" s="44"/>
@@ -12403,7 +12403,7 @@
       <c r="Q98" s="29"/>
       <c r="R98" s="69"/>
       <c r="S98" s="42"/>
-      <c r="T98" s="100"/>
+      <c r="T98" s="102"/>
       <c r="U98" s="44"/>
       <c r="V98" s="44"/>
       <c r="W98" s="45"/>
@@ -12423,7 +12423,7 @@
       <c r="AK98" s="68"/>
     </row>
     <row r="99" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="100"/>
+      <c r="A99" s="102"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="2"/>
@@ -12442,7 +12442,7 @@
       <c r="Q99" s="29"/>
       <c r="R99" s="68"/>
       <c r="S99" s="42"/>
-      <c r="T99" s="100"/>
+      <c r="T99" s="102"/>
       <c r="U99" s="44"/>
       <c r="V99" s="44"/>
       <c r="W99" s="45"/>
@@ -12462,7 +12462,7 @@
       <c r="AK99" s="68"/>
     </row>
     <row r="100" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="100"/>
+      <c r="A100" s="102"/>
       <c r="B100" s="55"/>
       <c r="C100" s="44"/>
       <c r="D100" s="45"/>
@@ -12481,7 +12481,7 @@
       <c r="Q100" s="29"/>
       <c r="R100" s="68"/>
       <c r="S100" s="42"/>
-      <c r="T100" s="100"/>
+      <c r="T100" s="102"/>
       <c r="U100" s="44"/>
       <c r="V100" s="44"/>
       <c r="W100" s="45"/>
@@ -12501,7 +12501,7 @@
       <c r="AK100" s="68"/>
     </row>
     <row r="101" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="100"/>
+      <c r="A101" s="102"/>
       <c r="B101" s="55"/>
       <c r="C101" s="44"/>
       <c r="D101" s="45"/>
@@ -12520,7 +12520,7 @@
       <c r="Q101" s="29"/>
       <c r="R101" s="68"/>
       <c r="S101" s="42"/>
-      <c r="T101" s="100"/>
+      <c r="T101" s="102"/>
       <c r="U101" s="44"/>
       <c r="V101" s="44"/>
       <c r="W101" s="45"/>
@@ -12540,7 +12540,7 @@
       <c r="AK101" s="68"/>
     </row>
     <row r="102" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="100"/>
+      <c r="A102" s="102"/>
       <c r="B102" s="44"/>
       <c r="C102" s="44"/>
       <c r="D102" s="45"/>
@@ -12559,7 +12559,7 @@
       <c r="Q102" s="29"/>
       <c r="R102" s="68"/>
       <c r="S102" s="42"/>
-      <c r="T102" s="100"/>
+      <c r="T102" s="102"/>
       <c r="U102" s="44"/>
       <c r="V102" s="44"/>
       <c r="W102" s="45"/>
@@ -12579,7 +12579,7 @@
       <c r="AK102" s="68"/>
     </row>
     <row r="103" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="100"/>
+      <c r="A103" s="102"/>
       <c r="B103" s="44"/>
       <c r="C103" s="44"/>
       <c r="D103" s="45"/>
@@ -12598,7 +12598,7 @@
       <c r="Q103" s="29"/>
       <c r="R103" s="68"/>
       <c r="S103" s="42"/>
-      <c r="T103" s="100"/>
+      <c r="T103" s="102"/>
       <c r="U103" s="54"/>
       <c r="V103" s="52"/>
       <c r="W103" s="52"/>
@@ -12618,7 +12618,7 @@
       <c r="AK103" s="68"/>
     </row>
     <row r="104" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="100"/>
+      <c r="A104" s="102"/>
       <c r="B104" s="44"/>
       <c r="C104" s="44"/>
       <c r="D104" s="45"/>
@@ -12637,7 +12637,7 @@
       <c r="Q104" s="29"/>
       <c r="R104" s="68"/>
       <c r="S104" s="42"/>
-      <c r="T104" s="100"/>
+      <c r="T104" s="102"/>
       <c r="U104" s="44"/>
       <c r="V104" s="44"/>
       <c r="W104" s="45"/>
@@ -12657,7 +12657,7 @@
       <c r="AK104" s="68"/>
     </row>
     <row r="105" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="100"/>
+      <c r="A105" s="102"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="2"/>
@@ -12676,7 +12676,7 @@
       <c r="Q105" s="29"/>
       <c r="R105" s="68"/>
       <c r="S105" s="42"/>
-      <c r="T105" s="100"/>
+      <c r="T105" s="102"/>
       <c r="U105" s="35"/>
       <c r="V105" s="1"/>
       <c r="W105" s="2"/>
@@ -12696,7 +12696,7 @@
       <c r="AK105" s="68"/>
     </row>
     <row r="106" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="100"/>
+      <c r="A106" s="102"/>
       <c r="B106" s="44"/>
       <c r="C106" s="44"/>
       <c r="D106" s="44"/>
@@ -12715,7 +12715,7 @@
       <c r="Q106" s="29"/>
       <c r="R106" s="68"/>
       <c r="S106" s="42"/>
-      <c r="T106" s="100"/>
+      <c r="T106" s="102"/>
       <c r="U106" s="35"/>
       <c r="V106" s="1"/>
       <c r="W106" s="2"/>
@@ -12735,7 +12735,7 @@
       <c r="AK106" s="68"/>
     </row>
     <row r="107" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="100"/>
+      <c r="A107" s="102"/>
       <c r="B107" s="44"/>
       <c r="C107" s="44"/>
       <c r="D107" s="45"/>
@@ -12754,7 +12754,7 @@
       <c r="Q107" s="29"/>
       <c r="R107" s="68"/>
       <c r="S107" s="42"/>
-      <c r="T107" s="100"/>
+      <c r="T107" s="102"/>
       <c r="U107" s="35"/>
       <c r="V107" s="1"/>
       <c r="W107" s="2"/>
@@ -12774,7 +12774,7 @@
       <c r="AK107" s="68"/>
     </row>
     <row r="108" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="100"/>
+      <c r="A108" s="102"/>
       <c r="B108" s="48"/>
       <c r="C108" s="49"/>
       <c r="D108" s="49"/>
@@ -12793,7 +12793,7 @@
       <c r="Q108" s="29"/>
       <c r="R108" s="68"/>
       <c r="S108" s="42"/>
-      <c r="T108" s="100"/>
+      <c r="T108" s="102"/>
       <c r="U108" s="35"/>
       <c r="V108" s="1"/>
       <c r="W108" s="2"/>
@@ -12813,7 +12813,7 @@
       <c r="AK108" s="68"/>
     </row>
     <row r="109" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="100"/>
+      <c r="A109" s="102"/>
       <c r="B109" s="44"/>
       <c r="C109" s="44"/>
       <c r="D109" s="44"/>
@@ -12832,7 +12832,7 @@
       <c r="Q109" s="29"/>
       <c r="R109" s="68"/>
       <c r="S109" s="42"/>
-      <c r="T109" s="100"/>
+      <c r="T109" s="102"/>
       <c r="U109" s="35"/>
       <c r="V109" s="1"/>
       <c r="W109" s="2"/>
@@ -12852,7 +12852,7 @@
       <c r="AK109" s="68"/>
     </row>
     <row r="110" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="100"/>
+      <c r="A110" s="102"/>
       <c r="B110" s="44"/>
       <c r="C110" s="44"/>
       <c r="D110" s="44"/>
@@ -12871,7 +12871,7 @@
       <c r="Q110" s="29"/>
       <c r="R110" s="68"/>
       <c r="S110" s="42"/>
-      <c r="T110" s="100"/>
+      <c r="T110" s="102"/>
       <c r="U110" s="35"/>
       <c r="V110" s="1"/>
       <c r="W110" s="2"/>
@@ -12891,7 +12891,7 @@
       <c r="AK110" s="68"/>
     </row>
     <row r="111" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="100"/>
+      <c r="A111" s="102"/>
       <c r="B111" s="44"/>
       <c r="C111" s="44"/>
       <c r="D111" s="44"/>
@@ -12910,7 +12910,7 @@
       <c r="Q111" s="29"/>
       <c r="R111" s="68"/>
       <c r="S111" s="42"/>
-      <c r="T111" s="100"/>
+      <c r="T111" s="102"/>
       <c r="U111" s="35"/>
       <c r="V111" s="1"/>
       <c r="W111" s="2"/>
@@ -12930,7 +12930,7 @@
       <c r="AK111" s="68"/>
     </row>
     <row r="112" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="100"/>
+      <c r="A112" s="102"/>
       <c r="B112" s="44"/>
       <c r="C112" s="44"/>
       <c r="D112" s="44"/>
@@ -12949,7 +12949,7 @@
       <c r="Q112" s="29"/>
       <c r="R112" s="68"/>
       <c r="S112" s="42"/>
-      <c r="T112" s="100"/>
+      <c r="T112" s="102"/>
       <c r="U112" s="35"/>
       <c r="V112" s="1"/>
       <c r="W112" s="2"/>
@@ -12969,7 +12969,7 @@
       <c r="AK112" s="68"/>
     </row>
     <row r="113" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="100"/>
+      <c r="A113" s="102"/>
       <c r="B113" s="44"/>
       <c r="C113" s="44"/>
       <c r="D113" s="44"/>
@@ -12988,7 +12988,7 @@
       <c r="Q113" s="29"/>
       <c r="R113" s="68"/>
       <c r="S113" s="42"/>
-      <c r="T113" s="100"/>
+      <c r="T113" s="102"/>
       <c r="U113" s="35"/>
       <c r="V113" s="1"/>
       <c r="W113" s="2"/>
@@ -13008,7 +13008,7 @@
       <c r="AK113" s="68"/>
     </row>
     <row r="114" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="100"/>
+      <c r="A114" s="102"/>
       <c r="B114" s="44"/>
       <c r="C114" s="44"/>
       <c r="D114" s="44"/>
@@ -13027,7 +13027,7 @@
       <c r="Q114" s="29"/>
       <c r="R114" s="68"/>
       <c r="S114" s="42"/>
-      <c r="T114" s="100"/>
+      <c r="T114" s="102"/>
       <c r="U114" s="35"/>
       <c r="V114" s="1"/>
       <c r="W114" s="2"/>
@@ -13047,7 +13047,7 @@
       <c r="AK114" s="68"/>
     </row>
     <row r="115" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="100"/>
+      <c r="A115" s="102"/>
       <c r="B115" s="44"/>
       <c r="C115" s="44"/>
       <c r="D115" s="44"/>
@@ -13066,7 +13066,7 @@
       <c r="Q115" s="29"/>
       <c r="R115" s="68"/>
       <c r="S115" s="42"/>
-      <c r="T115" s="100"/>
+      <c r="T115" s="102"/>
       <c r="U115" s="35"/>
       <c r="V115" s="1"/>
       <c r="W115" s="2"/>
@@ -13086,7 +13086,7 @@
       <c r="AK115" s="68"/>
     </row>
     <row r="116" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="100"/>
+      <c r="A116" s="102"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
@@ -13105,7 +13105,7 @@
       <c r="Q116" s="29"/>
       <c r="R116" s="68"/>
       <c r="S116" s="42"/>
-      <c r="T116" s="100"/>
+      <c r="T116" s="102"/>
       <c r="U116" s="35"/>
       <c r="V116" s="1"/>
       <c r="W116" s="2"/>
@@ -13125,7 +13125,7 @@
       <c r="AK116" s="68"/>
     </row>
     <row r="117" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="100"/>
+      <c r="A117" s="102"/>
       <c r="B117" s="44"/>
       <c r="C117" s="44"/>
       <c r="D117" s="45"/>
@@ -13144,7 +13144,7 @@
       <c r="Q117" s="29"/>
       <c r="R117" s="68"/>
       <c r="S117" s="42"/>
-      <c r="T117" s="100"/>
+      <c r="T117" s="102"/>
       <c r="U117" s="35"/>
       <c r="V117" s="1"/>
       <c r="W117" s="2"/>
@@ -13164,7 +13164,7 @@
       <c r="AK117" s="68"/>
     </row>
     <row r="118" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="100"/>
+      <c r="A118" s="102"/>
       <c r="B118" s="44"/>
       <c r="C118" s="44"/>
       <c r="D118" s="45"/>
@@ -13183,7 +13183,7 @@
       <c r="Q118" s="29"/>
       <c r="R118" s="68"/>
       <c r="S118" s="42"/>
-      <c r="T118" s="100"/>
+      <c r="T118" s="102"/>
       <c r="U118" s="35"/>
       <c r="V118" s="1"/>
       <c r="W118" s="2"/>
@@ -13203,7 +13203,7 @@
       <c r="AK118" s="68"/>
     </row>
     <row r="119" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="100"/>
+      <c r="A119" s="102"/>
       <c r="B119" s="47"/>
       <c r="C119" s="44"/>
       <c r="D119" s="45"/>
@@ -13222,7 +13222,7 @@
       <c r="Q119" s="29"/>
       <c r="R119" s="68"/>
       <c r="S119" s="42"/>
-      <c r="T119" s="100"/>
+      <c r="T119" s="102"/>
       <c r="U119" s="35"/>
       <c r="V119" s="1"/>
       <c r="W119" s="2"/>
@@ -13242,7 +13242,7 @@
       <c r="AK119" s="68"/>
     </row>
     <row r="120" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="100"/>
+      <c r="A120" s="102"/>
       <c r="B120" s="44"/>
       <c r="C120" s="44"/>
       <c r="D120" s="45"/>
@@ -13261,7 +13261,7 @@
       <c r="Q120" s="29"/>
       <c r="R120" s="68"/>
       <c r="S120" s="42"/>
-      <c r="T120" s="104"/>
+      <c r="T120" s="106"/>
       <c r="U120" s="35"/>
       <c r="V120" s="1"/>
       <c r="W120" s="2"/>
@@ -13327,21 +13327,21 @@
       <c r="V123" s="23"/>
       <c r="W123" s="23"/>
       <c r="X123" s="23"/>
-      <c r="Y123" s="85" t="s">
+      <c r="Y123" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="Z123" s="85"/>
-      <c r="AA123" s="85"/>
-      <c r="AB123" s="86" t="s">
+      <c r="Z123" s="89"/>
+      <c r="AA123" s="89"/>
+      <c r="AB123" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="AC123" s="86"/>
-      <c r="AD123" s="86"/>
-      <c r="AE123" s="87" t="s">
+      <c r="AC123" s="90"/>
+      <c r="AD123" s="90"/>
+      <c r="AE123" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="AF123" s="87"/>
-      <c r="AG123" s="87"/>
+      <c r="AF123" s="91"/>
+      <c r="AG123" s="91"/>
       <c r="AH123" s="88" t="s">
         <v>19</v>
       </c>
@@ -13355,21 +13355,21 @@
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
       <c r="E124" s="14"/>
-      <c r="F124" s="85" t="s">
+      <c r="F124" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="G124" s="85"/>
-      <c r="H124" s="85"/>
-      <c r="I124" s="86" t="s">
+      <c r="G124" s="89"/>
+      <c r="H124" s="89"/>
+      <c r="I124" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="J124" s="86"/>
-      <c r="K124" s="86"/>
-      <c r="L124" s="87" t="s">
+      <c r="J124" s="90"/>
+      <c r="K124" s="90"/>
+      <c r="L124" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="M124" s="87"/>
-      <c r="N124" s="87"/>
+      <c r="M124" s="91"/>
+      <c r="N124" s="91"/>
       <c r="O124" s="88" t="s">
         <v>19</v>
       </c>
@@ -13378,26 +13378,26 @@
       <c r="R124" s="36"/>
       <c r="S124" s="37"/>
       <c r="U124" s="19"/>
-      <c r="Y124" s="89" t="s">
+      <c r="Y124" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="Z124" s="90"/>
-      <c r="AA124" s="91"/>
-      <c r="AB124" s="89" t="s">
+      <c r="Z124" s="86"/>
+      <c r="AA124" s="87"/>
+      <c r="AB124" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="AC124" s="90"/>
-      <c r="AD124" s="91"/>
-      <c r="AE124" s="89" t="s">
+      <c r="AC124" s="86"/>
+      <c r="AD124" s="87"/>
+      <c r="AE124" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="AF124" s="90"/>
-      <c r="AG124" s="91"/>
-      <c r="AH124" s="89" t="s">
+      <c r="AF124" s="86"/>
+      <c r="AG124" s="87"/>
+      <c r="AH124" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="AI124" s="90"/>
-      <c r="AJ124" s="91"/>
+      <c r="AI124" s="86"/>
+      <c r="AJ124" s="87"/>
       <c r="AK124" s="36"/>
     </row>
     <row r="125" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -13407,26 +13407,26 @@
       <c r="B125" s="21"/>
       <c r="C125" s="21"/>
       <c r="D125" s="21"/>
-      <c r="F125" s="89" t="s">
+      <c r="F125" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="G125" s="90"/>
-      <c r="H125" s="91"/>
-      <c r="I125" s="89" t="s">
+      <c r="G125" s="86"/>
+      <c r="H125" s="87"/>
+      <c r="I125" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="J125" s="90"/>
-      <c r="K125" s="91"/>
-      <c r="L125" s="89" t="s">
+      <c r="J125" s="86"/>
+      <c r="K125" s="87"/>
+      <c r="L125" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="M125" s="90"/>
-      <c r="N125" s="91"/>
-      <c r="O125" s="89" t="s">
+      <c r="M125" s="86"/>
+      <c r="N125" s="87"/>
+      <c r="O125" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="P125" s="90"/>
-      <c r="Q125" s="91"/>
+      <c r="P125" s="86"/>
+      <c r="Q125" s="87"/>
       <c r="R125" s="36"/>
       <c r="S125" s="38"/>
       <c r="T125" s="18" t="s">
@@ -13485,7 +13485,7 @@
       </c>
     </row>
     <row r="126" spans="1:37" s="17" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="92" t="s">
+      <c r="A126" s="109" t="s">
         <v>30</v>
       </c>
       <c r="B126" s="18" t="s">
@@ -13540,7 +13540,7 @@
         <v>20</v>
       </c>
       <c r="S126" s="42"/>
-      <c r="T126" s="92" t="s">
+      <c r="T126" s="109" t="s">
         <v>30</v>
       </c>
       <c r="U126" s="44"/>
@@ -13562,7 +13562,7 @@
       <c r="AK126" s="79"/>
     </row>
     <row r="127" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A127" s="93"/>
+      <c r="A127" s="110"/>
       <c r="B127" s="44"/>
       <c r="C127" s="44"/>
       <c r="D127" s="45"/>
@@ -13581,7 +13581,7 @@
       <c r="Q127" s="29"/>
       <c r="R127" s="79"/>
       <c r="S127" s="42"/>
-      <c r="T127" s="93"/>
+      <c r="T127" s="110"/>
       <c r="U127" s="44"/>
       <c r="V127" s="44"/>
       <c r="W127" s="45"/>
@@ -13601,7 +13601,7 @@
       <c r="AK127" s="68"/>
     </row>
     <row r="128" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="93"/>
+      <c r="A128" s="110"/>
       <c r="B128" s="44"/>
       <c r="C128" s="44"/>
       <c r="D128" s="45"/>
@@ -13620,7 +13620,7 @@
       <c r="Q128" s="29"/>
       <c r="R128" s="68"/>
       <c r="S128" s="42"/>
-      <c r="T128" s="93"/>
+      <c r="T128" s="110"/>
       <c r="U128" s="54"/>
       <c r="V128" s="52"/>
       <c r="W128" s="52"/>
@@ -13640,7 +13640,7 @@
       <c r="AK128" s="68"/>
     </row>
     <row r="129" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="93"/>
+      <c r="A129" s="110"/>
       <c r="B129" s="53"/>
       <c r="C129" s="53"/>
       <c r="D129" s="65"/>
@@ -13659,7 +13659,7 @@
       <c r="Q129" s="29"/>
       <c r="R129" s="68"/>
       <c r="S129" s="42"/>
-      <c r="T129" s="93"/>
+      <c r="T129" s="110"/>
       <c r="U129" s="44"/>
       <c r="V129" s="44"/>
       <c r="W129" s="45"/>
@@ -13679,7 +13679,7 @@
       <c r="AK129" s="68"/>
     </row>
     <row r="130" spans="1:37" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="93"/>
+      <c r="A130" s="110"/>
       <c r="B130" s="44"/>
       <c r="C130" s="44"/>
       <c r="D130" s="44"/>
@@ -13698,7 +13698,7 @@
       <c r="Q130" s="29"/>
       <c r="R130" s="68"/>
       <c r="S130" s="43"/>
-      <c r="T130" s="93"/>
+      <c r="T130" s="110"/>
       <c r="U130" s="44"/>
       <c r="V130" s="44"/>
       <c r="W130" s="45"/>
@@ -13718,7 +13718,7 @@
       <c r="AK130" s="69"/>
     </row>
     <row r="131" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="93"/>
+      <c r="A131" s="110"/>
       <c r="B131" s="47"/>
       <c r="C131" s="44"/>
       <c r="D131" s="45"/>
@@ -13737,7 +13737,7 @@
       <c r="Q131" s="29"/>
       <c r="R131" s="69"/>
       <c r="S131" s="42"/>
-      <c r="T131" s="93"/>
+      <c r="T131" s="110"/>
       <c r="U131" s="54"/>
       <c r="V131" s="52"/>
       <c r="W131" s="52"/>
@@ -13757,7 +13757,7 @@
       <c r="AK131" s="68"/>
     </row>
     <row r="132" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A132" s="93"/>
+      <c r="A132" s="110"/>
       <c r="B132" s="44"/>
       <c r="C132" s="44"/>
       <c r="D132" s="45"/>
@@ -13776,7 +13776,7 @@
       <c r="Q132" s="29"/>
       <c r="R132" s="68"/>
       <c r="S132" s="42"/>
-      <c r="T132" s="93"/>
+      <c r="T132" s="110"/>
       <c r="U132" s="44"/>
       <c r="V132" s="44"/>
       <c r="W132" s="45"/>
@@ -13796,7 +13796,7 @@
       <c r="AK132" s="68"/>
     </row>
     <row r="133" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A133" s="93"/>
+      <c r="A133" s="110"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="2"/>
@@ -13815,7 +13815,7 @@
       <c r="Q133" s="29"/>
       <c r="R133" s="68"/>
       <c r="S133" s="42"/>
-      <c r="T133" s="93"/>
+      <c r="T133" s="110"/>
       <c r="U133" s="35"/>
       <c r="V133" s="1"/>
       <c r="W133" s="2"/>
@@ -13835,7 +13835,7 @@
       <c r="AK133" s="68"/>
     </row>
     <row r="134" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="93"/>
+      <c r="A134" s="110"/>
       <c r="B134" s="44"/>
       <c r="C134" s="44"/>
       <c r="D134" s="44"/>
@@ -13854,7 +13854,7 @@
       <c r="Q134" s="29"/>
       <c r="R134" s="68"/>
       <c r="S134" s="42"/>
-      <c r="T134" s="93"/>
+      <c r="T134" s="110"/>
       <c r="U134" s="35"/>
       <c r="V134" s="1"/>
       <c r="W134" s="2"/>
@@ -13874,7 +13874,7 @@
       <c r="AK134" s="68"/>
     </row>
     <row r="135" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="93"/>
+      <c r="A135" s="110"/>
       <c r="B135" s="44"/>
       <c r="C135" s="44"/>
       <c r="D135" s="45"/>
@@ -13893,7 +13893,7 @@
       <c r="Q135" s="29"/>
       <c r="R135" s="68"/>
       <c r="S135" s="42"/>
-      <c r="T135" s="93"/>
+      <c r="T135" s="110"/>
       <c r="U135" s="35"/>
       <c r="V135" s="1"/>
       <c r="W135" s="2"/>
@@ -13913,7 +13913,7 @@
       <c r="AK135" s="68"/>
     </row>
     <row r="136" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="93"/>
+      <c r="A136" s="110"/>
       <c r="B136" s="48"/>
       <c r="C136" s="49"/>
       <c r="D136" s="49"/>
@@ -13932,7 +13932,7 @@
       <c r="Q136" s="29"/>
       <c r="R136" s="68"/>
       <c r="S136" s="42"/>
-      <c r="T136" s="93"/>
+      <c r="T136" s="110"/>
       <c r="U136" s="35"/>
       <c r="V136" s="1"/>
       <c r="W136" s="2"/>
@@ -13952,7 +13952,7 @@
       <c r="AK136" s="68"/>
     </row>
     <row r="137" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="93"/>
+      <c r="A137" s="110"/>
       <c r="B137" s="44"/>
       <c r="C137" s="44"/>
       <c r="D137" s="44"/>
@@ -13971,7 +13971,7 @@
       <c r="Q137" s="29"/>
       <c r="R137" s="68"/>
       <c r="S137" s="42"/>
-      <c r="T137" s="93"/>
+      <c r="T137" s="110"/>
       <c r="U137" s="35"/>
       <c r="V137" s="1"/>
       <c r="W137" s="2"/>
@@ -13991,7 +13991,7 @@
       <c r="AK137" s="68"/>
     </row>
     <row r="138" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="93"/>
+      <c r="A138" s="110"/>
       <c r="B138" s="44"/>
       <c r="C138" s="44"/>
       <c r="D138" s="44"/>
@@ -14010,7 +14010,7 @@
       <c r="Q138" s="29"/>
       <c r="R138" s="68"/>
       <c r="S138" s="42"/>
-      <c r="T138" s="93"/>
+      <c r="T138" s="110"/>
       <c r="U138" s="35"/>
       <c r="V138" s="1"/>
       <c r="W138" s="2"/>
@@ -14030,7 +14030,7 @@
       <c r="AK138" s="68"/>
     </row>
     <row r="139" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="93"/>
+      <c r="A139" s="110"/>
       <c r="B139" s="44"/>
       <c r="C139" s="44"/>
       <c r="D139" s="44"/>
@@ -14049,7 +14049,7 @@
       <c r="Q139" s="29"/>
       <c r="R139" s="68"/>
       <c r="S139" s="42"/>
-      <c r="T139" s="93"/>
+      <c r="T139" s="110"/>
       <c r="U139" s="35"/>
       <c r="V139" s="1"/>
       <c r="W139" s="2"/>
@@ -14069,7 +14069,7 @@
       <c r="AK139" s="68"/>
     </row>
     <row r="140" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="93"/>
+      <c r="A140" s="110"/>
       <c r="B140" s="44"/>
       <c r="C140" s="44"/>
       <c r="D140" s="44"/>
@@ -14088,7 +14088,7 @@
       <c r="Q140" s="29"/>
       <c r="R140" s="68"/>
       <c r="S140" s="42"/>
-      <c r="T140" s="93"/>
+      <c r="T140" s="110"/>
       <c r="U140" s="35"/>
       <c r="V140" s="1"/>
       <c r="W140" s="2"/>
@@ -14108,7 +14108,7 @@
       <c r="AK140" s="68"/>
     </row>
     <row r="141" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="93"/>
+      <c r="A141" s="110"/>
       <c r="B141" s="44"/>
       <c r="C141" s="44"/>
       <c r="D141" s="44"/>
@@ -14127,7 +14127,7 @@
       <c r="Q141" s="29"/>
       <c r="R141" s="68"/>
       <c r="S141" s="42"/>
-      <c r="T141" s="93"/>
+      <c r="T141" s="110"/>
       <c r="U141" s="35"/>
       <c r="V141" s="1"/>
       <c r="W141" s="2"/>
@@ -14147,7 +14147,7 @@
       <c r="AK141" s="68"/>
     </row>
     <row r="142" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A142" s="93"/>
+      <c r="A142" s="110"/>
       <c r="B142" s="44"/>
       <c r="C142" s="44"/>
       <c r="D142" s="44"/>
@@ -14166,7 +14166,7 @@
       <c r="Q142" s="29"/>
       <c r="R142" s="68"/>
       <c r="S142" s="42"/>
-      <c r="T142" s="93"/>
+      <c r="T142" s="110"/>
       <c r="U142" s="35"/>
       <c r="V142" s="1"/>
       <c r="W142" s="2"/>
@@ -14186,7 +14186,7 @@
       <c r="AK142" s="68"/>
     </row>
     <row r="143" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A143" s="93"/>
+      <c r="A143" s="110"/>
       <c r="B143" s="44"/>
       <c r="C143" s="44"/>
       <c r="D143" s="44"/>
@@ -14205,7 +14205,7 @@
       <c r="Q143" s="29"/>
       <c r="R143" s="68"/>
       <c r="S143" s="42"/>
-      <c r="T143" s="93"/>
+      <c r="T143" s="110"/>
       <c r="U143" s="35"/>
       <c r="V143" s="1"/>
       <c r="W143" s="2"/>
@@ -14225,7 +14225,7 @@
       <c r="AK143" s="68"/>
     </row>
     <row r="144" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="93"/>
+      <c r="A144" s="110"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
@@ -14244,7 +14244,7 @@
       <c r="Q144" s="29"/>
       <c r="R144" s="68"/>
       <c r="S144" s="42"/>
-      <c r="T144" s="93"/>
+      <c r="T144" s="110"/>
       <c r="U144" s="35"/>
       <c r="V144" s="1"/>
       <c r="W144" s="2"/>
@@ -14264,7 +14264,7 @@
       <c r="AK144" s="68"/>
     </row>
     <row r="145" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="93"/>
+      <c r="A145" s="110"/>
       <c r="B145" s="44"/>
       <c r="C145" s="44"/>
       <c r="D145" s="45"/>
@@ -14283,7 +14283,7 @@
       <c r="Q145" s="29"/>
       <c r="R145" s="68"/>
       <c r="S145" s="42"/>
-      <c r="T145" s="93"/>
+      <c r="T145" s="110"/>
       <c r="U145" s="35"/>
       <c r="V145" s="1"/>
       <c r="W145" s="2"/>
@@ -14303,7 +14303,7 @@
       <c r="AK145" s="68"/>
     </row>
     <row r="146" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A146" s="93"/>
+      <c r="A146" s="110"/>
       <c r="B146" s="44"/>
       <c r="C146" s="44"/>
       <c r="D146" s="45"/>
@@ -14322,7 +14322,7 @@
       <c r="Q146" s="29"/>
       <c r="R146" s="68"/>
       <c r="S146" s="42"/>
-      <c r="T146" s="93"/>
+      <c r="T146" s="110"/>
       <c r="U146" s="35"/>
       <c r="V146" s="1"/>
       <c r="W146" s="2"/>
@@ -14342,7 +14342,7 @@
       <c r="AK146" s="68"/>
     </row>
     <row r="147" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A147" s="93"/>
+      <c r="A147" s="110"/>
       <c r="B147" s="47"/>
       <c r="C147" s="44"/>
       <c r="D147" s="45"/>
@@ -14361,7 +14361,7 @@
       <c r="Q147" s="29"/>
       <c r="R147" s="68"/>
       <c r="S147" s="42"/>
-      <c r="T147" s="93"/>
+      <c r="T147" s="110"/>
       <c r="U147" s="35"/>
       <c r="V147" s="1"/>
       <c r="W147" s="2"/>
@@ -14381,7 +14381,7 @@
       <c r="AK147" s="68"/>
     </row>
     <row r="148" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A148" s="93"/>
+      <c r="A148" s="110"/>
       <c r="B148" s="44"/>
       <c r="C148" s="44"/>
       <c r="D148" s="45"/>
@@ -14400,7 +14400,7 @@
       <c r="Q148" s="29"/>
       <c r="R148" s="68"/>
       <c r="S148" s="42"/>
-      <c r="T148" s="93"/>
+      <c r="T148" s="110"/>
       <c r="U148" s="35"/>
       <c r="V148" s="1"/>
       <c r="W148" s="2"/>
@@ -14446,21 +14446,21 @@
       <c r="V153" s="23"/>
       <c r="W153" s="23"/>
       <c r="X153" s="23"/>
-      <c r="Y153" s="85" t="s">
+      <c r="Y153" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="Z153" s="85"/>
-      <c r="AA153" s="85"/>
-      <c r="AB153" s="86" t="s">
+      <c r="Z153" s="89"/>
+      <c r="AA153" s="89"/>
+      <c r="AB153" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="AC153" s="86"/>
-      <c r="AD153" s="86"/>
-      <c r="AE153" s="87" t="s">
+      <c r="AC153" s="90"/>
+      <c r="AD153" s="90"/>
+      <c r="AE153" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="AF153" s="87"/>
-      <c r="AG153" s="87"/>
+      <c r="AF153" s="91"/>
+      <c r="AG153" s="91"/>
       <c r="AH153" s="88" t="s">
         <v>19</v>
       </c>
@@ -14474,21 +14474,21 @@
       <c r="C154" s="7"/>
       <c r="D154" s="7"/>
       <c r="E154" s="14"/>
-      <c r="F154" s="85" t="s">
+      <c r="F154" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="G154" s="85"/>
-      <c r="H154" s="85"/>
-      <c r="I154" s="86" t="s">
+      <c r="G154" s="89"/>
+      <c r="H154" s="89"/>
+      <c r="I154" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="J154" s="86"/>
-      <c r="K154" s="86"/>
-      <c r="L154" s="87" t="s">
+      <c r="J154" s="90"/>
+      <c r="K154" s="90"/>
+      <c r="L154" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="M154" s="87"/>
-      <c r="N154" s="87"/>
+      <c r="M154" s="91"/>
+      <c r="N154" s="91"/>
       <c r="O154" s="88" t="s">
         <v>19</v>
       </c>
@@ -14501,26 +14501,26 @@
       <c r="V154" s="17"/>
       <c r="W154" s="17"/>
       <c r="X154" s="17"/>
-      <c r="Y154" s="89" t="s">
+      <c r="Y154" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="Z154" s="90"/>
-      <c r="AA154" s="91"/>
-      <c r="AB154" s="89" t="s">
+      <c r="Z154" s="86"/>
+      <c r="AA154" s="87"/>
+      <c r="AB154" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="AC154" s="90"/>
-      <c r="AD154" s="91"/>
-      <c r="AE154" s="89" t="s">
+      <c r="AC154" s="86"/>
+      <c r="AD154" s="87"/>
+      <c r="AE154" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="AF154" s="90"/>
-      <c r="AG154" s="91"/>
-      <c r="AH154" s="89" t="s">
+      <c r="AF154" s="86"/>
+      <c r="AG154" s="87"/>
+      <c r="AH154" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="AI154" s="90"/>
-      <c r="AJ154" s="91"/>
+      <c r="AI154" s="86"/>
+      <c r="AJ154" s="87"/>
       <c r="AK154" s="36"/>
     </row>
     <row r="155" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -14531,26 +14531,26 @@
       <c r="C155" s="21"/>
       <c r="D155" s="21"/>
       <c r="E155" s="17"/>
-      <c r="F155" s="89" t="s">
+      <c r="F155" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="G155" s="90"/>
-      <c r="H155" s="91"/>
-      <c r="I155" s="89" t="s">
+      <c r="G155" s="86"/>
+      <c r="H155" s="87"/>
+      <c r="I155" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="J155" s="90"/>
-      <c r="K155" s="91"/>
-      <c r="L155" s="89" t="s">
+      <c r="J155" s="86"/>
+      <c r="K155" s="87"/>
+      <c r="L155" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="M155" s="90"/>
-      <c r="N155" s="91"/>
-      <c r="O155" s="89" t="s">
+      <c r="M155" s="86"/>
+      <c r="N155" s="87"/>
+      <c r="O155" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="P155" s="90"/>
-      <c r="Q155" s="91"/>
+      <c r="P155" s="86"/>
+      <c r="Q155" s="87"/>
       <c r="R155" s="36"/>
       <c r="S155" s="38"/>
       <c r="T155" s="18" t="s">
@@ -14609,7 +14609,7 @@
       </c>
     </row>
     <row r="156" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A156" s="94" t="s">
+      <c r="A156" s="107" t="s">
         <v>32</v>
       </c>
       <c r="B156" s="18" t="s">
@@ -14664,7 +14664,7 @@
         <v>20</v>
       </c>
       <c r="S156" s="42"/>
-      <c r="T156" s="94" t="s">
+      <c r="T156" s="107" t="s">
         <v>32</v>
       </c>
       <c r="U156" s="44"/>
@@ -14686,7 +14686,7 @@
       <c r="AK156" s="79"/>
     </row>
     <row r="157" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A157" s="95"/>
+      <c r="A157" s="108"/>
       <c r="B157" s="44"/>
       <c r="C157" s="44"/>
       <c r="D157" s="45"/>
@@ -14705,7 +14705,7 @@
       <c r="Q157" s="29"/>
       <c r="R157" s="79"/>
       <c r="S157" s="42"/>
-      <c r="T157" s="95"/>
+      <c r="T157" s="108"/>
       <c r="U157" s="44"/>
       <c r="V157" s="44"/>
       <c r="W157" s="45"/>
@@ -14725,7 +14725,7 @@
       <c r="AK157" s="68"/>
     </row>
     <row r="158" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A158" s="95"/>
+      <c r="A158" s="108"/>
       <c r="B158" s="44"/>
       <c r="C158" s="44"/>
       <c r="D158" s="45"/>
@@ -14744,7 +14744,7 @@
       <c r="Q158" s="29"/>
       <c r="R158" s="68"/>
       <c r="S158" s="42"/>
-      <c r="T158" s="95"/>
+      <c r="T158" s="108"/>
       <c r="U158" s="54"/>
       <c r="V158" s="52"/>
       <c r="W158" s="52"/>
@@ -14764,7 +14764,7 @@
       <c r="AK158" s="68"/>
     </row>
     <row r="159" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A159" s="95"/>
+      <c r="A159" s="108"/>
       <c r="B159" s="53"/>
       <c r="C159" s="53"/>
       <c r="D159" s="65"/>
@@ -14783,7 +14783,7 @@
       <c r="Q159" s="29"/>
       <c r="R159" s="68"/>
       <c r="S159" s="42"/>
-      <c r="T159" s="95"/>
+      <c r="T159" s="108"/>
       <c r="U159" s="44"/>
       <c r="V159" s="44"/>
       <c r="W159" s="45"/>
@@ -14803,7 +14803,7 @@
       <c r="AK159" s="68"/>
     </row>
     <row r="160" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A160" s="95"/>
+      <c r="A160" s="108"/>
       <c r="B160" s="44"/>
       <c r="C160" s="44"/>
       <c r="D160" s="44"/>
@@ -14822,7 +14822,7 @@
       <c r="Q160" s="29"/>
       <c r="R160" s="68"/>
       <c r="S160" s="43"/>
-      <c r="T160" s="95"/>
+      <c r="T160" s="108"/>
       <c r="U160" s="44"/>
       <c r="V160" s="44"/>
       <c r="W160" s="45"/>
@@ -14842,7 +14842,7 @@
       <c r="AK160" s="69"/>
     </row>
     <row r="161" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A161" s="95"/>
+      <c r="A161" s="108"/>
       <c r="B161" s="47"/>
       <c r="C161" s="44"/>
       <c r="D161" s="45"/>
@@ -14861,7 +14861,7 @@
       <c r="Q161" s="29"/>
       <c r="R161" s="69"/>
       <c r="S161" s="42"/>
-      <c r="T161" s="95"/>
+      <c r="T161" s="108"/>
       <c r="U161" s="54"/>
       <c r="V161" s="52"/>
       <c r="W161" s="52"/>
@@ -14881,7 +14881,7 @@
       <c r="AK161" s="68"/>
     </row>
     <row r="162" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A162" s="95"/>
+      <c r="A162" s="108"/>
       <c r="B162" s="44"/>
       <c r="C162" s="44"/>
       <c r="D162" s="45"/>
@@ -14900,7 +14900,7 @@
       <c r="Q162" s="29"/>
       <c r="R162" s="68"/>
       <c r="S162" s="42"/>
-      <c r="T162" s="95"/>
+      <c r="T162" s="108"/>
       <c r="U162" s="44"/>
       <c r="V162" s="44"/>
       <c r="W162" s="45"/>
@@ -14920,7 +14920,7 @@
       <c r="AK162" s="68"/>
     </row>
     <row r="163" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A163" s="95"/>
+      <c r="A163" s="108"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
       <c r="D163" s="2"/>
@@ -14939,7 +14939,7 @@
       <c r="Q163" s="29"/>
       <c r="R163" s="68"/>
       <c r="S163" s="42"/>
-      <c r="T163" s="95"/>
+      <c r="T163" s="108"/>
       <c r="U163" s="35"/>
       <c r="V163" s="1"/>
       <c r="W163" s="2"/>
@@ -14959,7 +14959,7 @@
       <c r="AK163" s="68"/>
     </row>
     <row r="164" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A164" s="95"/>
+      <c r="A164" s="108"/>
       <c r="B164" s="44"/>
       <c r="C164" s="44"/>
       <c r="D164" s="44"/>
@@ -14978,7 +14978,7 @@
       <c r="Q164" s="29"/>
       <c r="R164" s="68"/>
       <c r="S164" s="42"/>
-      <c r="T164" s="95"/>
+      <c r="T164" s="108"/>
       <c r="U164" s="35"/>
       <c r="V164" s="1"/>
       <c r="W164" s="2"/>
@@ -14998,7 +14998,7 @@
       <c r="AK164" s="68"/>
     </row>
     <row r="165" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A165" s="95"/>
+      <c r="A165" s="108"/>
       <c r="B165" s="44"/>
       <c r="C165" s="44"/>
       <c r="D165" s="45"/>
@@ -15017,7 +15017,7 @@
       <c r="Q165" s="29"/>
       <c r="R165" s="68"/>
       <c r="S165" s="42"/>
-      <c r="T165" s="95"/>
+      <c r="T165" s="108"/>
       <c r="U165" s="35"/>
       <c r="V165" s="1"/>
       <c r="W165" s="2"/>
@@ -15037,7 +15037,7 @@
       <c r="AK165" s="68"/>
     </row>
     <row r="166" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A166" s="95"/>
+      <c r="A166" s="108"/>
       <c r="B166" s="48"/>
       <c r="C166" s="49"/>
       <c r="D166" s="49"/>
@@ -15056,7 +15056,7 @@
       <c r="Q166" s="29"/>
       <c r="R166" s="68"/>
       <c r="S166" s="42"/>
-      <c r="T166" s="95"/>
+      <c r="T166" s="108"/>
       <c r="U166" s="35"/>
       <c r="V166" s="1"/>
       <c r="W166" s="2"/>
@@ -15076,7 +15076,7 @@
       <c r="AK166" s="68"/>
     </row>
     <row r="167" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A167" s="95"/>
+      <c r="A167" s="108"/>
       <c r="B167" s="44"/>
       <c r="C167" s="44"/>
       <c r="D167" s="44"/>
@@ -15095,7 +15095,7 @@
       <c r="Q167" s="29"/>
       <c r="R167" s="68"/>
       <c r="S167" s="42"/>
-      <c r="T167" s="95"/>
+      <c r="T167" s="108"/>
       <c r="U167" s="35"/>
       <c r="V167" s="1"/>
       <c r="W167" s="2"/>
@@ -15115,7 +15115,7 @@
       <c r="AK167" s="68"/>
     </row>
     <row r="168" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A168" s="95"/>
+      <c r="A168" s="108"/>
       <c r="B168" s="44"/>
       <c r="C168" s="44"/>
       <c r="D168" s="44"/>
@@ -15134,7 +15134,7 @@
       <c r="Q168" s="29"/>
       <c r="R168" s="68"/>
       <c r="S168" s="42"/>
-      <c r="T168" s="95"/>
+      <c r="T168" s="108"/>
       <c r="U168" s="35"/>
       <c r="V168" s="1"/>
       <c r="W168" s="2"/>
@@ -15154,7 +15154,7 @@
       <c r="AK168" s="68"/>
     </row>
     <row r="169" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A169" s="95"/>
+      <c r="A169" s="108"/>
       <c r="B169" s="44"/>
       <c r="C169" s="44"/>
       <c r="D169" s="44"/>
@@ -15173,7 +15173,7 @@
       <c r="Q169" s="29"/>
       <c r="R169" s="68"/>
       <c r="S169" s="42"/>
-      <c r="T169" s="95"/>
+      <c r="T169" s="108"/>
       <c r="U169" s="35"/>
       <c r="V169" s="1"/>
       <c r="W169" s="2"/>
@@ -15193,7 +15193,7 @@
       <c r="AK169" s="68"/>
     </row>
     <row r="170" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A170" s="95"/>
+      <c r="A170" s="108"/>
       <c r="B170" s="44"/>
       <c r="C170" s="44"/>
       <c r="D170" s="44"/>
@@ -15212,7 +15212,7 @@
       <c r="Q170" s="29"/>
       <c r="R170" s="68"/>
       <c r="S170" s="42"/>
-      <c r="T170" s="95"/>
+      <c r="T170" s="108"/>
       <c r="U170" s="35"/>
       <c r="V170" s="1"/>
       <c r="W170" s="2"/>
@@ -15232,7 +15232,7 @@
       <c r="AK170" s="68"/>
     </row>
     <row r="171" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A171" s="95"/>
+      <c r="A171" s="108"/>
       <c r="B171" s="44"/>
       <c r="C171" s="44"/>
       <c r="D171" s="44"/>
@@ -15251,7 +15251,7 @@
       <c r="Q171" s="29"/>
       <c r="R171" s="68"/>
       <c r="S171" s="42"/>
-      <c r="T171" s="95"/>
+      <c r="T171" s="108"/>
       <c r="U171" s="35"/>
       <c r="V171" s="1"/>
       <c r="W171" s="2"/>
@@ -15271,7 +15271,7 @@
       <c r="AK171" s="68"/>
     </row>
     <row r="172" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A172" s="95"/>
+      <c r="A172" s="108"/>
       <c r="B172" s="44"/>
       <c r="C172" s="44"/>
       <c r="D172" s="44"/>
@@ -15290,7 +15290,7 @@
       <c r="Q172" s="29"/>
       <c r="R172" s="68"/>
       <c r="S172" s="42"/>
-      <c r="T172" s="95"/>
+      <c r="T172" s="108"/>
       <c r="U172" s="35"/>
       <c r="V172" s="1"/>
       <c r="W172" s="2"/>
@@ -15310,7 +15310,7 @@
       <c r="AK172" s="68"/>
     </row>
     <row r="173" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A173" s="95"/>
+      <c r="A173" s="108"/>
       <c r="B173" s="44"/>
       <c r="C173" s="44"/>
       <c r="D173" s="44"/>
@@ -15329,7 +15329,7 @@
       <c r="Q173" s="29"/>
       <c r="R173" s="68"/>
       <c r="S173" s="42"/>
-      <c r="T173" s="95"/>
+      <c r="T173" s="108"/>
       <c r="U173" s="35"/>
       <c r="V173" s="1"/>
       <c r="W173" s="2"/>
@@ -15349,7 +15349,7 @@
       <c r="AK173" s="68"/>
     </row>
     <row r="174" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A174" s="95"/>
+      <c r="A174" s="108"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
       <c r="D174" s="1"/>
@@ -15368,7 +15368,7 @@
       <c r="Q174" s="29"/>
       <c r="R174" s="68"/>
       <c r="S174" s="42"/>
-      <c r="T174" s="95"/>
+      <c r="T174" s="108"/>
       <c r="U174" s="35"/>
       <c r="V174" s="1"/>
       <c r="W174" s="2"/>
@@ -15388,7 +15388,7 @@
       <c r="AK174" s="68"/>
     </row>
     <row r="175" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A175" s="95"/>
+      <c r="A175" s="108"/>
       <c r="B175" s="44"/>
       <c r="C175" s="44"/>
       <c r="D175" s="45"/>
@@ -15407,7 +15407,7 @@
       <c r="Q175" s="29"/>
       <c r="R175" s="68"/>
       <c r="S175" s="42"/>
-      <c r="T175" s="95"/>
+      <c r="T175" s="108"/>
       <c r="U175" s="35"/>
       <c r="V175" s="1"/>
       <c r="W175" s="2"/>
@@ -15427,7 +15427,7 @@
       <c r="AK175" s="68"/>
     </row>
     <row r="176" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A176" s="95"/>
+      <c r="A176" s="108"/>
       <c r="B176" s="44"/>
       <c r="C176" s="44"/>
       <c r="D176" s="45"/>
@@ -15446,7 +15446,7 @@
       <c r="Q176" s="29"/>
       <c r="R176" s="68"/>
       <c r="S176" s="42"/>
-      <c r="T176" s="95"/>
+      <c r="T176" s="108"/>
       <c r="U176" s="35"/>
       <c r="V176" s="1"/>
       <c r="W176" s="2"/>
@@ -15466,7 +15466,7 @@
       <c r="AK176" s="68"/>
     </row>
     <row r="177" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A177" s="95"/>
+      <c r="A177" s="108"/>
       <c r="B177" s="47"/>
       <c r="C177" s="44"/>
       <c r="D177" s="45"/>
@@ -15485,7 +15485,7 @@
       <c r="Q177" s="29"/>
       <c r="R177" s="68"/>
       <c r="S177" s="42"/>
-      <c r="T177" s="95"/>
+      <c r="T177" s="108"/>
       <c r="U177" s="35"/>
       <c r="V177" s="1"/>
       <c r="W177" s="2"/>
@@ -15505,7 +15505,7 @@
       <c r="AK177" s="68"/>
     </row>
     <row r="178" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A178" s="95"/>
+      <c r="A178" s="108"/>
       <c r="B178" s="44"/>
       <c r="C178" s="44"/>
       <c r="D178" s="45"/>
@@ -15524,7 +15524,7 @@
       <c r="Q178" s="29"/>
       <c r="R178" s="68"/>
       <c r="S178" s="42"/>
-      <c r="T178" s="95"/>
+      <c r="T178" s="108"/>
       <c r="U178" s="35"/>
       <c r="V178" s="1"/>
       <c r="W178" s="2"/>
@@ -15564,24 +15564,66 @@
     </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="AH85:AJ85"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="AH43:AJ43"/>
-    <mergeCell ref="AH44:AJ44"/>
-    <mergeCell ref="AH84:AJ84"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="O43:Q43"/>
-    <mergeCell ref="O44:Q44"/>
-    <mergeCell ref="O85:Q85"/>
-    <mergeCell ref="I86:K86"/>
-    <mergeCell ref="L86:N86"/>
-    <mergeCell ref="O86:Q86"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F85:H85"/>
-    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="Y153:AA153"/>
+    <mergeCell ref="AB153:AD153"/>
+    <mergeCell ref="AE153:AG153"/>
+    <mergeCell ref="AH153:AJ153"/>
+    <mergeCell ref="F155:H155"/>
+    <mergeCell ref="I155:K155"/>
+    <mergeCell ref="L155:N155"/>
+    <mergeCell ref="O155:Q155"/>
+    <mergeCell ref="Y154:AA154"/>
+    <mergeCell ref="AB154:AD154"/>
+    <mergeCell ref="AE154:AG154"/>
+    <mergeCell ref="AH154:AJ154"/>
+    <mergeCell ref="A126:A148"/>
+    <mergeCell ref="T126:T148"/>
+    <mergeCell ref="F154:H154"/>
+    <mergeCell ref="I154:K154"/>
+    <mergeCell ref="L154:N154"/>
+    <mergeCell ref="O154:Q154"/>
+    <mergeCell ref="A156:A178"/>
+    <mergeCell ref="T156:T178"/>
+    <mergeCell ref="AB123:AD123"/>
+    <mergeCell ref="AE123:AG123"/>
+    <mergeCell ref="AH123:AJ123"/>
+    <mergeCell ref="F125:H125"/>
+    <mergeCell ref="I125:K125"/>
+    <mergeCell ref="L125:N125"/>
+    <mergeCell ref="O125:Q125"/>
+    <mergeCell ref="Y124:AA124"/>
+    <mergeCell ref="AB124:AD124"/>
+    <mergeCell ref="AE124:AG124"/>
+    <mergeCell ref="AH124:AJ124"/>
+    <mergeCell ref="F124:H124"/>
+    <mergeCell ref="I124:K124"/>
+    <mergeCell ref="L124:N124"/>
+    <mergeCell ref="O124:Q124"/>
+    <mergeCell ref="Y123:AA123"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="A87:A120"/>
+    <mergeCell ref="T46:T82"/>
+    <mergeCell ref="T87:T120"/>
+    <mergeCell ref="I85:K85"/>
+    <mergeCell ref="L85:N85"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="AE3:AG3"/>
+    <mergeCell ref="AE43:AG43"/>
+    <mergeCell ref="T3:W3"/>
+    <mergeCell ref="AB43:AD43"/>
+    <mergeCell ref="AB2:AD2"/>
+    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="Y3:AA3"/>
+    <mergeCell ref="T5:T41"/>
     <mergeCell ref="AB84:AD84"/>
     <mergeCell ref="AE84:AG84"/>
     <mergeCell ref="AB85:AD85"/>
@@ -15598,66 +15640,24 @@
     <mergeCell ref="Y44:AA44"/>
     <mergeCell ref="Y84:AA84"/>
     <mergeCell ref="Y85:AA85"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="AE3:AG3"/>
-    <mergeCell ref="AE43:AG43"/>
-    <mergeCell ref="T3:W3"/>
-    <mergeCell ref="AB43:AD43"/>
-    <mergeCell ref="AB2:AD2"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="Y3:AA3"/>
-    <mergeCell ref="T5:T41"/>
-    <mergeCell ref="O124:Q124"/>
-    <mergeCell ref="Y123:AA123"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="A87:A120"/>
-    <mergeCell ref="T46:T82"/>
-    <mergeCell ref="T87:T120"/>
-    <mergeCell ref="I85:K85"/>
-    <mergeCell ref="L85:N85"/>
-    <mergeCell ref="A156:A178"/>
-    <mergeCell ref="T156:T178"/>
-    <mergeCell ref="AB123:AD123"/>
-    <mergeCell ref="AE123:AG123"/>
-    <mergeCell ref="AH123:AJ123"/>
-    <mergeCell ref="F125:H125"/>
-    <mergeCell ref="I125:K125"/>
-    <mergeCell ref="L125:N125"/>
-    <mergeCell ref="O125:Q125"/>
-    <mergeCell ref="Y124:AA124"/>
-    <mergeCell ref="AB124:AD124"/>
-    <mergeCell ref="AE124:AG124"/>
-    <mergeCell ref="AH124:AJ124"/>
-    <mergeCell ref="F124:H124"/>
-    <mergeCell ref="I124:K124"/>
-    <mergeCell ref="L124:N124"/>
-    <mergeCell ref="A126:A148"/>
-    <mergeCell ref="T126:T148"/>
-    <mergeCell ref="F154:H154"/>
-    <mergeCell ref="I154:K154"/>
-    <mergeCell ref="L154:N154"/>
-    <mergeCell ref="O154:Q154"/>
-    <mergeCell ref="Y153:AA153"/>
-    <mergeCell ref="AB153:AD153"/>
-    <mergeCell ref="AE153:AG153"/>
-    <mergeCell ref="AH153:AJ153"/>
-    <mergeCell ref="F155:H155"/>
-    <mergeCell ref="I155:K155"/>
-    <mergeCell ref="L155:N155"/>
-    <mergeCell ref="O155:Q155"/>
-    <mergeCell ref="Y154:AA154"/>
-    <mergeCell ref="AB154:AD154"/>
-    <mergeCell ref="AE154:AG154"/>
-    <mergeCell ref="AH154:AJ154"/>
+    <mergeCell ref="I86:K86"/>
+    <mergeCell ref="L86:N86"/>
+    <mergeCell ref="O86:Q86"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="O43:Q43"/>
+    <mergeCell ref="O44:Q44"/>
+    <mergeCell ref="O85:Q85"/>
+    <mergeCell ref="AH85:AJ85"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="AH3:AJ3"/>
+    <mergeCell ref="AH43:AJ43"/>
+    <mergeCell ref="AH44:AJ44"/>
+    <mergeCell ref="AH84:AJ84"/>
   </mergeCells>
   <conditionalFormatting sqref="AB87:AG95 AB5:AG15 I88:N88 AB46:AG82 I62:L62 N62 I63:N84 I5:N42 I91:N91 I93:N96 I98:N116 I119:N121 I132:N144 AB131:AG148 O127:Q148 AH126:AJ147 F127:H149 Y126:AA148 O46:Q73 F46:H83 I46:N61">
     <cfRule type="containsText" dxfId="387" priority="936" operator="containsText" text="y">

</xml_diff>